<commit_message>
Remove Unused for Laporan and Laporan Follow Up
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
@@ -714,16 +714,25 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -741,17 +750,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1106,120 +1106,120 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
       <c r="AX2" s="12" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
     </row>
     <row r="4" spans="1:157" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
       <c r="AA5" s="20" t="s">
         <v>36</v>
       </c>
       <c r="AB5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AC5" s="25" t="s">
+      <c r="AC5" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25"/>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="25"/>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="33" t="s">
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="30"/>
+      <c r="AK5" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="AL5" s="33"/>
-      <c r="AM5" s="33"/>
-      <c r="AN5" s="33"/>
-      <c r="AO5" s="33"/>
-      <c r="AP5" s="33"/>
-      <c r="AQ5" s="33"/>
-      <c r="AR5" s="33"/>
-      <c r="AS5" s="33"/>
-      <c r="AT5" s="34" t="s">
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AU5" s="34"/>
-      <c r="AV5" s="34"/>
-      <c r="AW5" s="34"/>
+      <c r="AU5" s="29"/>
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="29"/>
       <c r="AX5" s="27" t="s">
         <v>139</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="FA5" s="23"/>
     </row>
     <row r="6" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="11"/>
@@ -1387,19 +1387,19 @@
       <c r="AY6" s="21"/>
       <c r="AZ6" s="21"/>
       <c r="BA6" s="21"/>
-      <c r="BB6" s="24" t="s">
+      <c r="BB6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="BC6" s="24"/>
-      <c r="BD6" s="24" t="s">
+      <c r="BC6" s="26"/>
+      <c r="BD6" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="BE6" s="24"/>
-      <c r="BF6" s="24" t="s">
+      <c r="BE6" s="26"/>
+      <c r="BF6" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="BG6" s="24"/>
-      <c r="BH6" s="24"/>
+      <c r="BG6" s="26"/>
+      <c r="BH6" s="26"/>
       <c r="BI6" s="21"/>
       <c r="BJ6" s="21"/>
       <c r="BK6" s="21"/>
@@ -1470,14 +1470,14 @@
       <c r="DX6" s="23"/>
       <c r="DY6" s="23"/>
       <c r="DZ6" s="23"/>
-      <c r="EA6" s="35" t="s">
+      <c r="EA6" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="EB6" s="35"/>
-      <c r="EC6" s="35"/>
-      <c r="ED6" s="35"/>
-      <c r="EE6" s="35"/>
-      <c r="EF6" s="36" t="s">
+      <c r="EB6" s="25"/>
+      <c r="EC6" s="25"/>
+      <c r="ED6" s="25"/>
+      <c r="EE6" s="25"/>
+      <c r="EF6" s="24" t="s">
         <v>103</v>
       </c>
       <c r="EG6" s="23"/>
@@ -1503,7 +1503,7 @@
       <c r="FA6" s="23"/>
     </row>
     <row r="7" spans="1:157" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
@@ -53245,11 +53245,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="EA6:EE6"/>
-    <mergeCell ref="BB6:BC6"/>
-    <mergeCell ref="BD6:BE6"/>
-    <mergeCell ref="BF6:BH6"/>
-    <mergeCell ref="AX5:BD5"/>
     <mergeCell ref="AK5:AS5"/>
     <mergeCell ref="AT5:AW5"/>
     <mergeCell ref="AC5:AJ5"/>
@@ -53259,6 +53254,11 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="D5:Z5"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="EA6:EE6"/>
+    <mergeCell ref="BB6:BC6"/>
+    <mergeCell ref="BD6:BE6"/>
+    <mergeCell ref="BF6:BH6"/>
+    <mergeCell ref="AX5:BD5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB : Laporan Follow Up - Pemeriksaan Laboratorium
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FA500"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BY8" sqref="BY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
OAB - Update template report Follow Up
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="153">
   <si>
     <t>No</t>
   </si>
@@ -430,9 +430,6 @@
     <t>Komplikasi Tindakan Invasive/Operasi</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Pemeriksaan Penunjang</t>
   </si>
   <si>
@@ -717,15 +714,6 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -751,6 +739,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1066,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FA500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BY8" sqref="BY8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,129 +1103,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
     </row>
     <row r="2" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="AX2" s="12" t="s">
-        <v>138</v>
-      </c>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
     </row>
     <row r="3" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
     </row>
     <row r="4" spans="1:157" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="35" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+      <c r="T5" s="32"/>
+      <c r="U5" s="32"/>
+      <c r="V5" s="32"/>
+      <c r="W5" s="32"/>
+      <c r="X5" s="32"/>
+      <c r="Y5" s="32"/>
+      <c r="Z5" s="32"/>
       <c r="AA5" s="20" t="s">
         <v>36</v>
       </c>
       <c r="AB5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AC5" s="30" t="s">
+      <c r="AC5" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="AD5" s="30"/>
-      <c r="AE5" s="30"/>
-      <c r="AF5" s="30"/>
-      <c r="AG5" s="30"/>
-      <c r="AH5" s="30"/>
-      <c r="AI5" s="30"/>
-      <c r="AJ5" s="30"/>
-      <c r="AK5" s="28" t="s">
+      <c r="AD5" s="27"/>
+      <c r="AE5" s="27"/>
+      <c r="AF5" s="27"/>
+      <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="28"/>
-      <c r="AN5" s="28"/>
-      <c r="AO5" s="28"/>
-      <c r="AP5" s="28"/>
-      <c r="AQ5" s="28"/>
-      <c r="AR5" s="28"/>
-      <c r="AS5" s="28"/>
-      <c r="AT5" s="29" t="s">
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="25"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
+      <c r="AR5" s="25"/>
+      <c r="AS5" s="25"/>
+      <c r="AT5" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="AU5" s="29"/>
-      <c r="AV5" s="29"/>
-      <c r="AW5" s="29"/>
-      <c r="AX5" s="27" t="s">
-        <v>139</v>
+      <c r="AU5" s="26"/>
+      <c r="AV5" s="26"/>
+      <c r="AW5" s="26"/>
+      <c r="AX5" s="36" t="s">
+        <v>138</v>
       </c>
-      <c r="AY5" s="27"/>
-      <c r="AZ5" s="27"/>
-      <c r="BA5" s="27"/>
-      <c r="BB5" s="27"/>
-      <c r="BC5" s="27"/>
-      <c r="BD5" s="27"/>
+      <c r="AY5" s="36"/>
+      <c r="AZ5" s="36"/>
+      <c r="BA5" s="36"/>
+      <c r="BB5" s="36"/>
+      <c r="BC5" s="36"/>
+      <c r="BD5" s="36"/>
       <c r="BE5" s="21"/>
       <c r="BF5" s="21"/>
       <c r="BG5" s="21"/>
@@ -1289,7 +1283,7 @@
       <c r="DJ5" s="21"/>
       <c r="DK5" s="21"/>
       <c r="DL5" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="DM5" s="23"/>
       <c r="DN5" s="23"/>
@@ -1334,7 +1328,7 @@
       <c r="FA5" s="23"/>
     </row>
     <row r="6" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="11"/>
@@ -1387,19 +1381,19 @@
       <c r="AY6" s="21"/>
       <c r="AZ6" s="21"/>
       <c r="BA6" s="21"/>
-      <c r="BB6" s="26" t="s">
+      <c r="BB6" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="BC6" s="26"/>
-      <c r="BD6" s="26" t="s">
+      <c r="BC6" s="35"/>
+      <c r="BD6" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="BE6" s="26"/>
-      <c r="BF6" s="26" t="s">
-        <v>142</v>
+      <c r="BE6" s="35"/>
+      <c r="BF6" s="35" t="s">
+        <v>141</v>
       </c>
-      <c r="BG6" s="26"/>
-      <c r="BH6" s="26"/>
+      <c r="BG6" s="35"/>
+      <c r="BH6" s="35"/>
       <c r="BI6" s="21"/>
       <c r="BJ6" s="21"/>
       <c r="BK6" s="21"/>
@@ -1470,13 +1464,13 @@
       <c r="DX6" s="23"/>
       <c r="DY6" s="23"/>
       <c r="DZ6" s="23"/>
-      <c r="EA6" s="25" t="s">
+      <c r="EA6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="EB6" s="25"/>
-      <c r="EC6" s="25"/>
-      <c r="ED6" s="25"/>
-      <c r="EE6" s="25"/>
+      <c r="EB6" s="34"/>
+      <c r="EC6" s="34"/>
+      <c r="ED6" s="34"/>
+      <c r="EE6" s="34"/>
       <c r="EF6" s="24" t="s">
         <v>103</v>
       </c>
@@ -1503,7 +1497,7 @@
       <c r="FA6" s="23"/>
     </row>
     <row r="7" spans="1:157" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
@@ -1649,10 +1643,10 @@
         <v>132</v>
       </c>
       <c r="AX7" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AY7" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AZ7" s="8" t="s">
         <v>61</v>
@@ -1682,7 +1676,7 @@
         <v>68</v>
       </c>
       <c r="BI7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="BJ7" s="7" t="s">
         <v>33</v>
@@ -1724,16 +1718,16 @@
         <v>109</v>
       </c>
       <c r="BW7" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="BX7" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="BX7" s="8" t="s">
+      <c r="BY7" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="BY7" s="8" t="s">
+      <c r="BZ7" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="BZ7" s="8" t="s">
-        <v>147</v>
       </c>
       <c r="CA7" s="8" t="s">
         <v>110</v>
@@ -1769,7 +1763,7 @@
         <v>119</v>
       </c>
       <c r="CL7" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="CM7" s="7" t="s">
         <v>33</v>
@@ -1847,7 +1841,7 @@
         <v>79</v>
       </c>
       <c r="DL7" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="DM7" s="5" t="s">
         <v>33</v>
@@ -1871,7 +1865,7 @@
         <v>85</v>
       </c>
       <c r="DT7" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="DU7" s="4" t="s">
         <v>96</v>
@@ -1910,7 +1904,7 @@
         <v>32</v>
       </c>
       <c r="EG7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="EH7" s="2" t="s">
         <v>33</v>
@@ -1952,7 +1946,7 @@
         <v>95</v>
       </c>
       <c r="EU7" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="EV7" s="10" t="s">
         <v>34</v>
@@ -53245,6 +53239,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="EA6:EE6"/>
+    <mergeCell ref="BB6:BC6"/>
+    <mergeCell ref="BD6:BE6"/>
+    <mergeCell ref="BF6:BH6"/>
+    <mergeCell ref="AX5:BD5"/>
     <mergeCell ref="AK5:AS5"/>
     <mergeCell ref="AT5:AW5"/>
     <mergeCell ref="AC5:AJ5"/>
@@ -53254,11 +53253,6 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="D5:Z5"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="EA6:EE6"/>
-    <mergeCell ref="BB6:BC6"/>
-    <mergeCell ref="BD6:BE6"/>
-    <mergeCell ref="BF6:BH6"/>
-    <mergeCell ref="AX5:BD5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
OAB - Update format column for template report Follow Up
</commit_message>
<xml_diff>
--- a/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
+++ b/Laravel-InaLUTS/resources/templates/Report_Follow_Up_OAB.xlsx
@@ -640,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -714,6 +714,15 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -741,14 +750,17 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1075,7 +1087,7 @@
     <col min="4" max="4" width="11.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="12" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="12" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="40" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="12" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="12" customWidth="1"/>
@@ -1103,126 +1115,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:157" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
     </row>
-    <row r="4" spans="1:157" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:157" s="3" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="37"/>
+    </row>
     <row r="5" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="32" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="32"/>
-      <c r="U5" s="32"/>
-      <c r="V5" s="32"/>
-      <c r="W5" s="32"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="35"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="35"/>
+      <c r="T5" s="35"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="35"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="35"/>
+      <c r="Y5" s="35"/>
+      <c r="Z5" s="35"/>
       <c r="AA5" s="20" t="s">
         <v>36</v>
       </c>
       <c r="AB5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AC5" s="27" t="s">
+      <c r="AC5" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="AD5" s="27"/>
-      <c r="AE5" s="27"/>
-      <c r="AF5" s="27"/>
-      <c r="AG5" s="27"/>
-      <c r="AH5" s="27"/>
-      <c r="AI5" s="27"/>
-      <c r="AJ5" s="27"/>
-      <c r="AK5" s="25" t="s">
+      <c r="AD5" s="30"/>
+      <c r="AE5" s="30"/>
+      <c r="AF5" s="30"/>
+      <c r="AG5" s="30"/>
+      <c r="AH5" s="30"/>
+      <c r="AI5" s="30"/>
+      <c r="AJ5" s="30"/>
+      <c r="AK5" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="25"/>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
-      <c r="AR5" s="25"/>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="26" t="s">
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="28"/>
+      <c r="AN5" s="28"/>
+      <c r="AO5" s="28"/>
+      <c r="AP5" s="28"/>
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="28"/>
+      <c r="AS5" s="28"/>
+      <c r="AT5" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="AU5" s="26"/>
-      <c r="AV5" s="26"/>
-      <c r="AW5" s="26"/>
-      <c r="AX5" s="36" t="s">
+      <c r="AU5" s="29"/>
+      <c r="AV5" s="29"/>
+      <c r="AW5" s="29"/>
+      <c r="AX5" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="AY5" s="36"/>
-      <c r="AZ5" s="36"/>
-      <c r="BA5" s="36"/>
-      <c r="BB5" s="36"/>
-      <c r="BC5" s="36"/>
-      <c r="BD5" s="36"/>
+      <c r="AY5" s="27"/>
+      <c r="AZ5" s="27"/>
+      <c r="BA5" s="27"/>
+      <c r="BB5" s="27"/>
+      <c r="BC5" s="27"/>
+      <c r="BD5" s="27"/>
       <c r="BE5" s="21"/>
       <c r="BF5" s="21"/>
       <c r="BG5" s="21"/>
@@ -1328,13 +1342,13 @@
       <c r="FA5" s="23"/>
     </row>
     <row r="6" spans="1:157" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="G6" s="38"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
       <c r="J6" s="11"/>
@@ -1381,19 +1395,19 @@
       <c r="AY6" s="21"/>
       <c r="AZ6" s="21"/>
       <c r="BA6" s="21"/>
-      <c r="BB6" s="35" t="s">
+      <c r="BB6" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="BC6" s="35"/>
-      <c r="BD6" s="35" t="s">
+      <c r="BC6" s="26"/>
+      <c r="BD6" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="BE6" s="35"/>
-      <c r="BF6" s="35" t="s">
+      <c r="BE6" s="26"/>
+      <c r="BF6" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="BG6" s="35"/>
-      <c r="BH6" s="35"/>
+      <c r="BG6" s="26"/>
+      <c r="BH6" s="26"/>
       <c r="BI6" s="21"/>
       <c r="BJ6" s="21"/>
       <c r="BK6" s="21"/>
@@ -1464,13 +1478,13 @@
       <c r="DX6" s="23"/>
       <c r="DY6" s="23"/>
       <c r="DZ6" s="23"/>
-      <c r="EA6" s="34" t="s">
+      <c r="EA6" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="EB6" s="34"/>
-      <c r="EC6" s="34"/>
-      <c r="ED6" s="34"/>
-      <c r="EE6" s="34"/>
+      <c r="EB6" s="25"/>
+      <c r="EC6" s="25"/>
+      <c r="ED6" s="25"/>
+      <c r="EE6" s="25"/>
       <c r="EF6" s="24" t="s">
         <v>103</v>
       </c>
@@ -1497,7 +1511,7 @@
       <c r="FA6" s="23"/>
     </row>
     <row r="7" spans="1:157" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="16" t="s">
         <v>13</v>
       </c>
@@ -1513,7 +1527,7 @@
       <c r="F7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="39" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1968,6 +1982,7 @@
     <row r="8" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="19"/>
       <c r="C8" s="19"/>
+      <c r="G8" s="40"/>
       <c r="BE8" s="22"/>
       <c r="BF8" s="22"/>
       <c r="BG8" s="22"/>
@@ -2072,6 +2087,7 @@
     <row r="9" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="19"/>
       <c r="C9" s="19"/>
+      <c r="G9" s="40"/>
       <c r="BE9" s="22"/>
       <c r="BF9" s="22"/>
       <c r="BG9" s="22"/>
@@ -2176,6 +2192,7 @@
     <row r="10" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
+      <c r="G10" s="40"/>
       <c r="BE10" s="22"/>
       <c r="BF10" s="22"/>
       <c r="BG10" s="22"/>
@@ -2280,6 +2297,7 @@
     <row r="11" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19"/>
       <c r="C11" s="19"/>
+      <c r="G11" s="40"/>
       <c r="BE11" s="22"/>
       <c r="BF11" s="22"/>
       <c r="BG11" s="22"/>
@@ -2384,6 +2402,7 @@
     <row r="12" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="19"/>
+      <c r="G12" s="40"/>
       <c r="BE12" s="22"/>
       <c r="BF12" s="22"/>
       <c r="BG12" s="22"/>
@@ -2488,6 +2507,7 @@
     <row r="13" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
       <c r="C13" s="19"/>
+      <c r="G13" s="40"/>
       <c r="BE13" s="22"/>
       <c r="BF13" s="22"/>
       <c r="BG13" s="22"/>
@@ -2592,6 +2612,7 @@
     <row r="14" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" s="19"/>
+      <c r="G14" s="40"/>
       <c r="BE14" s="22"/>
       <c r="BF14" s="22"/>
       <c r="BG14" s="22"/>
@@ -2696,6 +2717,7 @@
     <row r="15" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
       <c r="C15" s="19"/>
+      <c r="G15" s="40"/>
       <c r="BE15" s="22"/>
       <c r="BF15" s="22"/>
       <c r="BG15" s="22"/>
@@ -2800,6 +2822,7 @@
     <row r="16" spans="1:157" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
       <c r="C16" s="19"/>
+      <c r="G16" s="40"/>
       <c r="BE16" s="22"/>
       <c r="BF16" s="22"/>
       <c r="BG16" s="22"/>
@@ -2904,6 +2927,7 @@
     <row r="17" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
+      <c r="G17" s="40"/>
       <c r="BE17" s="22"/>
       <c r="BF17" s="22"/>
       <c r="BG17" s="22"/>
@@ -3008,6 +3032,7 @@
     <row r="18" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
+      <c r="G18" s="40"/>
       <c r="BE18" s="22"/>
       <c r="BF18" s="22"/>
       <c r="BG18" s="22"/>
@@ -3112,6 +3137,7 @@
     <row r="19" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
+      <c r="G19" s="40"/>
       <c r="BE19" s="22"/>
       <c r="BF19" s="22"/>
       <c r="BG19" s="22"/>
@@ -3216,6 +3242,7 @@
     <row r="20" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
+      <c r="G20" s="40"/>
       <c r="BE20" s="22"/>
       <c r="BF20" s="22"/>
       <c r="BG20" s="22"/>
@@ -3320,6 +3347,7 @@
     <row r="21" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
+      <c r="G21" s="40"/>
       <c r="BE21" s="22"/>
       <c r="BF21" s="22"/>
       <c r="BG21" s="22"/>
@@ -3424,6 +3452,7 @@
     <row r="22" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
+      <c r="G22" s="40"/>
       <c r="BE22" s="22"/>
       <c r="BF22" s="22"/>
       <c r="BG22" s="22"/>
@@ -3528,6 +3557,7 @@
     <row r="23" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
+      <c r="G23" s="40"/>
       <c r="BE23" s="22"/>
       <c r="BF23" s="22"/>
       <c r="BG23" s="22"/>
@@ -3632,6 +3662,7 @@
     <row r="24" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
+      <c r="G24" s="40"/>
       <c r="BE24" s="22"/>
       <c r="BF24" s="22"/>
       <c r="BG24" s="22"/>
@@ -3736,6 +3767,7 @@
     <row r="25" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
+      <c r="G25" s="40"/>
       <c r="BE25" s="22"/>
       <c r="BF25" s="22"/>
       <c r="BG25" s="22"/>
@@ -3840,6 +3872,7 @@
     <row r="26" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
+      <c r="G26" s="40"/>
       <c r="BE26" s="22"/>
       <c r="BF26" s="22"/>
       <c r="BG26" s="22"/>
@@ -3944,6 +3977,7 @@
     <row r="27" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
+      <c r="G27" s="40"/>
       <c r="BE27" s="22"/>
       <c r="BF27" s="22"/>
       <c r="BG27" s="22"/>
@@ -4048,6 +4082,7 @@
     <row r="28" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
+      <c r="G28" s="40"/>
       <c r="BE28" s="22"/>
       <c r="BF28" s="22"/>
       <c r="BG28" s="22"/>
@@ -4152,6 +4187,7 @@
     <row r="29" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
+      <c r="G29" s="40"/>
       <c r="BE29" s="22"/>
       <c r="BF29" s="22"/>
       <c r="BG29" s="22"/>
@@ -4256,6 +4292,7 @@
     <row r="30" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
+      <c r="G30" s="40"/>
       <c r="BE30" s="22"/>
       <c r="BF30" s="22"/>
       <c r="BG30" s="22"/>
@@ -4360,6 +4397,7 @@
     <row r="31" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
+      <c r="G31" s="40"/>
       <c r="BE31" s="22"/>
       <c r="BF31" s="22"/>
       <c r="BG31" s="22"/>
@@ -4464,6 +4502,7 @@
     <row r="32" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
+      <c r="G32" s="40"/>
       <c r="BE32" s="22"/>
       <c r="BF32" s="22"/>
       <c r="BG32" s="22"/>
@@ -4568,6 +4607,7 @@
     <row r="33" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
+      <c r="G33" s="40"/>
       <c r="BE33" s="22"/>
       <c r="BF33" s="22"/>
       <c r="BG33" s="22"/>
@@ -4672,6 +4712,7 @@
     <row r="34" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
+      <c r="G34" s="40"/>
       <c r="BE34" s="22"/>
       <c r="BF34" s="22"/>
       <c r="BG34" s="22"/>
@@ -4776,6 +4817,7 @@
     <row r="35" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
+      <c r="G35" s="40"/>
       <c r="BE35" s="22"/>
       <c r="BF35" s="22"/>
       <c r="BG35" s="22"/>
@@ -4880,6 +4922,7 @@
     <row r="36" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
+      <c r="G36" s="40"/>
       <c r="BE36" s="22"/>
       <c r="BF36" s="22"/>
       <c r="BG36" s="22"/>
@@ -4984,6 +5027,7 @@
     <row r="37" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
+      <c r="G37" s="40"/>
       <c r="BE37" s="22"/>
       <c r="BF37" s="22"/>
       <c r="BG37" s="22"/>
@@ -5088,6 +5132,7 @@
     <row r="38" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
+      <c r="G38" s="40"/>
       <c r="BE38" s="22"/>
       <c r="BF38" s="22"/>
       <c r="BG38" s="22"/>
@@ -5192,6 +5237,7 @@
     <row r="39" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
+      <c r="G39" s="40"/>
       <c r="BE39" s="22"/>
       <c r="BF39" s="22"/>
       <c r="BG39" s="22"/>
@@ -5296,6 +5342,7 @@
     <row r="40" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="19"/>
       <c r="C40" s="19"/>
+      <c r="G40" s="40"/>
       <c r="BE40" s="22"/>
       <c r="BF40" s="22"/>
       <c r="BG40" s="22"/>
@@ -5400,6 +5447,7 @@
     <row r="41" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
+      <c r="G41" s="40"/>
       <c r="BE41" s="22"/>
       <c r="BF41" s="22"/>
       <c r="BG41" s="22"/>
@@ -5504,6 +5552,7 @@
     <row r="42" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
+      <c r="G42" s="40"/>
       <c r="BE42" s="22"/>
       <c r="BF42" s="22"/>
       <c r="BG42" s="22"/>
@@ -5608,6 +5657,7 @@
     <row r="43" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
+      <c r="G43" s="40"/>
       <c r="BE43" s="22"/>
       <c r="BF43" s="22"/>
       <c r="BG43" s="22"/>
@@ -5712,6 +5762,7 @@
     <row r="44" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
+      <c r="G44" s="40"/>
       <c r="BE44" s="22"/>
       <c r="BF44" s="22"/>
       <c r="BG44" s="22"/>
@@ -5816,6 +5867,7 @@
     <row r="45" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
+      <c r="G45" s="40"/>
       <c r="BE45" s="22"/>
       <c r="BF45" s="22"/>
       <c r="BG45" s="22"/>
@@ -5920,6 +5972,7 @@
     <row r="46" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
+      <c r="G46" s="40"/>
       <c r="BE46" s="22"/>
       <c r="BF46" s="22"/>
       <c r="BG46" s="22"/>
@@ -6024,6 +6077,7 @@
     <row r="47" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
+      <c r="G47" s="40"/>
       <c r="BE47" s="22"/>
       <c r="BF47" s="22"/>
       <c r="BG47" s="22"/>
@@ -6128,6 +6182,7 @@
     <row r="48" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="19"/>
       <c r="C48" s="19"/>
+      <c r="G48" s="40"/>
       <c r="BE48" s="22"/>
       <c r="BF48" s="22"/>
       <c r="BG48" s="22"/>
@@ -6232,6 +6287,7 @@
     <row r="49" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="19"/>
       <c r="C49" s="19"/>
+      <c r="G49" s="40"/>
       <c r="BE49" s="22"/>
       <c r="BF49" s="22"/>
       <c r="BG49" s="22"/>
@@ -6336,6 +6392,7 @@
     <row r="50" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="19"/>
       <c r="C50" s="19"/>
+      <c r="G50" s="40"/>
       <c r="BE50" s="22"/>
       <c r="BF50" s="22"/>
       <c r="BG50" s="22"/>
@@ -6440,6 +6497,7 @@
     <row r="51" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="19"/>
       <c r="C51" s="19"/>
+      <c r="G51" s="40"/>
       <c r="BE51" s="22"/>
       <c r="BF51" s="22"/>
       <c r="BG51" s="22"/>
@@ -6544,6 +6602,7 @@
     <row r="52" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="19"/>
       <c r="C52" s="19"/>
+      <c r="G52" s="40"/>
       <c r="BE52" s="22"/>
       <c r="BF52" s="22"/>
       <c r="BG52" s="22"/>
@@ -6648,6 +6707,7 @@
     <row r="53" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="19"/>
       <c r="C53" s="19"/>
+      <c r="G53" s="40"/>
       <c r="BE53" s="22"/>
       <c r="BF53" s="22"/>
       <c r="BG53" s="22"/>
@@ -6752,6 +6812,7 @@
     <row r="54" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="19"/>
       <c r="C54" s="19"/>
+      <c r="G54" s="40"/>
       <c r="BE54" s="22"/>
       <c r="BF54" s="22"/>
       <c r="BG54" s="22"/>
@@ -6856,6 +6917,7 @@
     <row r="55" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="19"/>
       <c r="C55" s="19"/>
+      <c r="G55" s="40"/>
       <c r="BE55" s="22"/>
       <c r="BF55" s="22"/>
       <c r="BG55" s="22"/>
@@ -6960,6 +7022,7 @@
     <row r="56" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="19"/>
       <c r="C56" s="19"/>
+      <c r="G56" s="40"/>
       <c r="BE56" s="22"/>
       <c r="BF56" s="22"/>
       <c r="BG56" s="22"/>
@@ -7064,6 +7127,7 @@
     <row r="57" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="19"/>
       <c r="C57" s="19"/>
+      <c r="G57" s="40"/>
       <c r="BE57" s="22"/>
       <c r="BF57" s="22"/>
       <c r="BG57" s="22"/>
@@ -7168,6 +7232,7 @@
     <row r="58" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="19"/>
       <c r="C58" s="19"/>
+      <c r="G58" s="40"/>
       <c r="BE58" s="22"/>
       <c r="BF58" s="22"/>
       <c r="BG58" s="22"/>
@@ -7272,6 +7337,7 @@
     <row r="59" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="19"/>
       <c r="C59" s="19"/>
+      <c r="G59" s="40"/>
       <c r="BE59" s="22"/>
       <c r="BF59" s="22"/>
       <c r="BG59" s="22"/>
@@ -7376,6 +7442,7 @@
     <row r="60" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="19"/>
       <c r="C60" s="19"/>
+      <c r="G60" s="40"/>
       <c r="BE60" s="22"/>
       <c r="BF60" s="22"/>
       <c r="BG60" s="22"/>
@@ -7480,6 +7547,7 @@
     <row r="61" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="19"/>
       <c r="C61" s="19"/>
+      <c r="G61" s="40"/>
       <c r="BE61" s="22"/>
       <c r="BF61" s="22"/>
       <c r="BG61" s="22"/>
@@ -7584,6 +7652,7 @@
     <row r="62" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="19"/>
       <c r="C62" s="19"/>
+      <c r="G62" s="40"/>
       <c r="BE62" s="22"/>
       <c r="BF62" s="22"/>
       <c r="BG62" s="22"/>
@@ -7688,6 +7757,7 @@
     <row r="63" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="19"/>
       <c r="C63" s="19"/>
+      <c r="G63" s="40"/>
       <c r="BE63" s="22"/>
       <c r="BF63" s="22"/>
       <c r="BG63" s="22"/>
@@ -7792,6 +7862,7 @@
     <row r="64" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="19"/>
       <c r="C64" s="19"/>
+      <c r="G64" s="40"/>
       <c r="BE64" s="22"/>
       <c r="BF64" s="22"/>
       <c r="BG64" s="22"/>
@@ -7896,6 +7967,7 @@
     <row r="65" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="19"/>
       <c r="C65" s="19"/>
+      <c r="G65" s="40"/>
       <c r="BE65" s="22"/>
       <c r="BF65" s="22"/>
       <c r="BG65" s="22"/>
@@ -8000,6 +8072,7 @@
     <row r="66" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="19"/>
       <c r="C66" s="19"/>
+      <c r="G66" s="40"/>
       <c r="BE66" s="22"/>
       <c r="BF66" s="22"/>
       <c r="BG66" s="22"/>
@@ -8104,6 +8177,7 @@
     <row r="67" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="19"/>
       <c r="C67" s="19"/>
+      <c r="G67" s="40"/>
       <c r="BE67" s="22"/>
       <c r="BF67" s="22"/>
       <c r="BG67" s="22"/>
@@ -8208,6 +8282,7 @@
     <row r="68" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="19"/>
       <c r="C68" s="19"/>
+      <c r="G68" s="40"/>
       <c r="BE68" s="22"/>
       <c r="BF68" s="22"/>
       <c r="BG68" s="22"/>
@@ -8312,6 +8387,7 @@
     <row r="69" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="19"/>
       <c r="C69" s="19"/>
+      <c r="G69" s="40"/>
       <c r="BE69" s="22"/>
       <c r="BF69" s="22"/>
       <c r="BG69" s="22"/>
@@ -8416,6 +8492,7 @@
     <row r="70" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="19"/>
       <c r="C70" s="19"/>
+      <c r="G70" s="40"/>
       <c r="BE70" s="22"/>
       <c r="BF70" s="22"/>
       <c r="BG70" s="22"/>
@@ -8520,6 +8597,7 @@
     <row r="71" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="19"/>
       <c r="C71" s="19"/>
+      <c r="G71" s="40"/>
       <c r="BE71" s="22"/>
       <c r="BF71" s="22"/>
       <c r="BG71" s="22"/>
@@ -8624,6 +8702,7 @@
     <row r="72" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="19"/>
       <c r="C72" s="19"/>
+      <c r="G72" s="40"/>
       <c r="BE72" s="22"/>
       <c r="BF72" s="22"/>
       <c r="BG72" s="22"/>
@@ -8728,6 +8807,7 @@
     <row r="73" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="19"/>
       <c r="C73" s="19"/>
+      <c r="G73" s="40"/>
       <c r="BE73" s="22"/>
       <c r="BF73" s="22"/>
       <c r="BG73" s="22"/>
@@ -8832,6 +8912,7 @@
     <row r="74" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="19"/>
       <c r="C74" s="19"/>
+      <c r="G74" s="40"/>
       <c r="BE74" s="22"/>
       <c r="BF74" s="22"/>
       <c r="BG74" s="22"/>
@@ -8936,6 +9017,7 @@
     <row r="75" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="19"/>
       <c r="C75" s="19"/>
+      <c r="G75" s="40"/>
       <c r="BE75" s="22"/>
       <c r="BF75" s="22"/>
       <c r="BG75" s="22"/>
@@ -9040,6 +9122,7 @@
     <row r="76" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="19"/>
       <c r="C76" s="19"/>
+      <c r="G76" s="40"/>
       <c r="BE76" s="22"/>
       <c r="BF76" s="22"/>
       <c r="BG76" s="22"/>
@@ -9144,6 +9227,7 @@
     <row r="77" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
+      <c r="G77" s="40"/>
       <c r="BE77" s="22"/>
       <c r="BF77" s="22"/>
       <c r="BG77" s="22"/>
@@ -9248,6 +9332,7 @@
     <row r="78" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="19"/>
       <c r="C78" s="19"/>
+      <c r="G78" s="40"/>
       <c r="BE78" s="22"/>
       <c r="BF78" s="22"/>
       <c r="BG78" s="22"/>
@@ -9352,6 +9437,7 @@
     <row r="79" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="19"/>
       <c r="C79" s="19"/>
+      <c r="G79" s="40"/>
       <c r="BE79" s="22"/>
       <c r="BF79" s="22"/>
       <c r="BG79" s="22"/>
@@ -9456,6 +9542,7 @@
     <row r="80" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="19"/>
       <c r="C80" s="19"/>
+      <c r="G80" s="40"/>
       <c r="BE80" s="22"/>
       <c r="BF80" s="22"/>
       <c r="BG80" s="22"/>
@@ -9560,6 +9647,7 @@
     <row r="81" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="19"/>
       <c r="C81" s="19"/>
+      <c r="G81" s="40"/>
       <c r="BE81" s="22"/>
       <c r="BF81" s="22"/>
       <c r="BG81" s="22"/>
@@ -9664,6 +9752,7 @@
     <row r="82" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="19"/>
       <c r="C82" s="19"/>
+      <c r="G82" s="40"/>
       <c r="BE82" s="22"/>
       <c r="BF82" s="22"/>
       <c r="BG82" s="22"/>
@@ -9768,6 +9857,7 @@
     <row r="83" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="19"/>
       <c r="C83" s="19"/>
+      <c r="G83" s="40"/>
       <c r="BE83" s="22"/>
       <c r="BF83" s="22"/>
       <c r="BG83" s="22"/>
@@ -9872,6 +9962,7 @@
     <row r="84" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="19"/>
       <c r="C84" s="19"/>
+      <c r="G84" s="40"/>
       <c r="BE84" s="22"/>
       <c r="BF84" s="22"/>
       <c r="BG84" s="22"/>
@@ -9976,6 +10067,7 @@
     <row r="85" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="19"/>
       <c r="C85" s="19"/>
+      <c r="G85" s="40"/>
       <c r="BE85" s="22"/>
       <c r="BF85" s="22"/>
       <c r="BG85" s="22"/>
@@ -10080,6 +10172,7 @@
     <row r="86" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="19"/>
       <c r="C86" s="19"/>
+      <c r="G86" s="40"/>
       <c r="BE86" s="22"/>
       <c r="BF86" s="22"/>
       <c r="BG86" s="22"/>
@@ -10184,6 +10277,7 @@
     <row r="87" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="19"/>
       <c r="C87" s="19"/>
+      <c r="G87" s="40"/>
       <c r="BE87" s="22"/>
       <c r="BF87" s="22"/>
       <c r="BG87" s="22"/>
@@ -10288,6 +10382,7 @@
     <row r="88" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="19"/>
       <c r="C88" s="19"/>
+      <c r="G88" s="40"/>
       <c r="BE88" s="22"/>
       <c r="BF88" s="22"/>
       <c r="BG88" s="22"/>
@@ -10392,6 +10487,7 @@
     <row r="89" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="19"/>
       <c r="C89" s="19"/>
+      <c r="G89" s="40"/>
       <c r="BE89" s="22"/>
       <c r="BF89" s="22"/>
       <c r="BG89" s="22"/>
@@ -10496,6 +10592,7 @@
     <row r="90" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="19"/>
       <c r="C90" s="19"/>
+      <c r="G90" s="40"/>
       <c r="BE90" s="22"/>
       <c r="BF90" s="22"/>
       <c r="BG90" s="22"/>
@@ -10600,6 +10697,7 @@
     <row r="91" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="19"/>
       <c r="C91" s="19"/>
+      <c r="G91" s="40"/>
       <c r="BE91" s="22"/>
       <c r="BF91" s="22"/>
       <c r="BG91" s="22"/>
@@ -10704,6 +10802,7 @@
     <row r="92" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="19"/>
       <c r="C92" s="19"/>
+      <c r="G92" s="40"/>
       <c r="BE92" s="22"/>
       <c r="BF92" s="22"/>
       <c r="BG92" s="22"/>
@@ -10808,6 +10907,7 @@
     <row r="93" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="19"/>
       <c r="C93" s="19"/>
+      <c r="G93" s="40"/>
       <c r="BE93" s="22"/>
       <c r="BF93" s="22"/>
       <c r="BG93" s="22"/>
@@ -10912,6 +11012,7 @@
     <row r="94" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="19"/>
       <c r="C94" s="19"/>
+      <c r="G94" s="40"/>
       <c r="BE94" s="22"/>
       <c r="BF94" s="22"/>
       <c r="BG94" s="22"/>
@@ -11016,6 +11117,7 @@
     <row r="95" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="19"/>
       <c r="C95" s="19"/>
+      <c r="G95" s="40"/>
       <c r="BE95" s="22"/>
       <c r="BF95" s="22"/>
       <c r="BG95" s="22"/>
@@ -11120,6 +11222,7 @@
     <row r="96" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="19"/>
       <c r="C96" s="19"/>
+      <c r="G96" s="40"/>
       <c r="BE96" s="22"/>
       <c r="BF96" s="22"/>
       <c r="BG96" s="22"/>
@@ -11224,6 +11327,7 @@
     <row r="97" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="19"/>
       <c r="C97" s="19"/>
+      <c r="G97" s="40"/>
       <c r="BE97" s="22"/>
       <c r="BF97" s="22"/>
       <c r="BG97" s="22"/>
@@ -11328,6 +11432,7 @@
     <row r="98" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="19"/>
       <c r="C98" s="19"/>
+      <c r="G98" s="40"/>
       <c r="BE98" s="22"/>
       <c r="BF98" s="22"/>
       <c r="BG98" s="22"/>
@@ -11432,6 +11537,7 @@
     <row r="99" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="19"/>
       <c r="C99" s="19"/>
+      <c r="G99" s="40"/>
       <c r="BE99" s="22"/>
       <c r="BF99" s="22"/>
       <c r="BG99" s="22"/>
@@ -11536,6 +11642,7 @@
     <row r="100" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="19"/>
       <c r="C100" s="19"/>
+      <c r="G100" s="40"/>
       <c r="BE100" s="22"/>
       <c r="BF100" s="22"/>
       <c r="BG100" s="22"/>
@@ -11640,6 +11747,7 @@
     <row r="101" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="19"/>
       <c r="C101" s="19"/>
+      <c r="G101" s="40"/>
       <c r="BE101" s="22"/>
       <c r="BF101" s="22"/>
       <c r="BG101" s="22"/>
@@ -11744,6 +11852,7 @@
     <row r="102" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="19"/>
       <c r="C102" s="19"/>
+      <c r="G102" s="40"/>
       <c r="BE102" s="22"/>
       <c r="BF102" s="22"/>
       <c r="BG102" s="22"/>
@@ -11848,6 +11957,7 @@
     <row r="103" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="19"/>
       <c r="C103" s="19"/>
+      <c r="G103" s="40"/>
       <c r="BE103" s="22"/>
       <c r="BF103" s="22"/>
       <c r="BG103" s="22"/>
@@ -11952,6 +12062,7 @@
     <row r="104" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="19"/>
       <c r="C104" s="19"/>
+      <c r="G104" s="40"/>
       <c r="BE104" s="22"/>
       <c r="BF104" s="22"/>
       <c r="BG104" s="22"/>
@@ -12056,6 +12167,7 @@
     <row r="105" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="19"/>
       <c r="C105" s="19"/>
+      <c r="G105" s="40"/>
       <c r="BE105" s="22"/>
       <c r="BF105" s="22"/>
       <c r="BG105" s="22"/>
@@ -12160,6 +12272,7 @@
     <row r="106" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="19"/>
       <c r="C106" s="19"/>
+      <c r="G106" s="40"/>
       <c r="BE106" s="22"/>
       <c r="BF106" s="22"/>
       <c r="BG106" s="22"/>
@@ -12264,6 +12377,7 @@
     <row r="107" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="19"/>
       <c r="C107" s="19"/>
+      <c r="G107" s="40"/>
       <c r="BE107" s="22"/>
       <c r="BF107" s="22"/>
       <c r="BG107" s="22"/>
@@ -12368,6 +12482,7 @@
     <row r="108" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
+      <c r="G108" s="40"/>
       <c r="BE108" s="22"/>
       <c r="BF108" s="22"/>
       <c r="BG108" s="22"/>
@@ -12472,6 +12587,7 @@
     <row r="109" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
+      <c r="G109" s="40"/>
       <c r="BE109" s="22"/>
       <c r="BF109" s="22"/>
       <c r="BG109" s="22"/>
@@ -12576,6 +12692,7 @@
     <row r="110" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
+      <c r="G110" s="40"/>
       <c r="BE110" s="22"/>
       <c r="BF110" s="22"/>
       <c r="BG110" s="22"/>
@@ -12680,6 +12797,7 @@
     <row r="111" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
+      <c r="G111" s="40"/>
       <c r="BE111" s="22"/>
       <c r="BF111" s="22"/>
       <c r="BG111" s="22"/>
@@ -12784,6 +12902,7 @@
     <row r="112" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
+      <c r="G112" s="40"/>
       <c r="BE112" s="22"/>
       <c r="BF112" s="22"/>
       <c r="BG112" s="22"/>
@@ -12888,6 +13007,7 @@
     <row r="113" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
+      <c r="G113" s="40"/>
       <c r="BE113" s="22"/>
       <c r="BF113" s="22"/>
       <c r="BG113" s="22"/>
@@ -12992,6 +13112,7 @@
     <row r="114" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
+      <c r="G114" s="40"/>
       <c r="BE114" s="22"/>
       <c r="BF114" s="22"/>
       <c r="BG114" s="22"/>
@@ -13096,6 +13217,7 @@
     <row r="115" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
+      <c r="G115" s="40"/>
       <c r="BE115" s="22"/>
       <c r="BF115" s="22"/>
       <c r="BG115" s="22"/>
@@ -13200,6 +13322,7 @@
     <row r="116" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
+      <c r="G116" s="40"/>
       <c r="BE116" s="22"/>
       <c r="BF116" s="22"/>
       <c r="BG116" s="22"/>
@@ -13304,6 +13427,7 @@
     <row r="117" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
+      <c r="G117" s="40"/>
       <c r="BE117" s="22"/>
       <c r="BF117" s="22"/>
       <c r="BG117" s="22"/>
@@ -13408,6 +13532,7 @@
     <row r="118" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
+      <c r="G118" s="40"/>
       <c r="BE118" s="22"/>
       <c r="BF118" s="22"/>
       <c r="BG118" s="22"/>
@@ -13512,6 +13637,7 @@
     <row r="119" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="19"/>
       <c r="C119" s="19"/>
+      <c r="G119" s="40"/>
       <c r="BE119" s="22"/>
       <c r="BF119" s="22"/>
       <c r="BG119" s="22"/>
@@ -13616,6 +13742,7 @@
     <row r="120" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
+      <c r="G120" s="40"/>
       <c r="BE120" s="22"/>
       <c r="BF120" s="22"/>
       <c r="BG120" s="22"/>
@@ -13720,6 +13847,7 @@
     <row r="121" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
+      <c r="G121" s="40"/>
       <c r="BE121" s="22"/>
       <c r="BF121" s="22"/>
       <c r="BG121" s="22"/>
@@ -13824,6 +13952,7 @@
     <row r="122" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="19"/>
       <c r="C122" s="19"/>
+      <c r="G122" s="40"/>
       <c r="BE122" s="22"/>
       <c r="BF122" s="22"/>
       <c r="BG122" s="22"/>
@@ -13928,6 +14057,7 @@
     <row r="123" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
+      <c r="G123" s="40"/>
       <c r="BE123" s="22"/>
       <c r="BF123" s="22"/>
       <c r="BG123" s="22"/>
@@ -14032,6 +14162,7 @@
     <row r="124" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B124" s="19"/>
       <c r="C124" s="19"/>
+      <c r="G124" s="40"/>
       <c r="BE124" s="22"/>
       <c r="BF124" s="22"/>
       <c r="BG124" s="22"/>
@@ -14136,6 +14267,7 @@
     <row r="125" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="19"/>
       <c r="C125" s="19"/>
+      <c r="G125" s="40"/>
       <c r="BE125" s="22"/>
       <c r="BF125" s="22"/>
       <c r="BG125" s="22"/>
@@ -14240,6 +14372,7 @@
     <row r="126" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
+      <c r="G126" s="40"/>
       <c r="BE126" s="22"/>
       <c r="BF126" s="22"/>
       <c r="BG126" s="22"/>
@@ -14344,6 +14477,7 @@
     <row r="127" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
+      <c r="G127" s="40"/>
       <c r="BE127" s="22"/>
       <c r="BF127" s="22"/>
       <c r="BG127" s="22"/>
@@ -14448,6 +14582,7 @@
     <row r="128" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
+      <c r="G128" s="40"/>
       <c r="BE128" s="22"/>
       <c r="BF128" s="22"/>
       <c r="BG128" s="22"/>
@@ -14552,6 +14687,7 @@
     <row r="129" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
+      <c r="G129" s="40"/>
       <c r="BE129" s="22"/>
       <c r="BF129" s="22"/>
       <c r="BG129" s="22"/>
@@ -14656,6 +14792,7 @@
     <row r="130" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
+      <c r="G130" s="40"/>
       <c r="BE130" s="22"/>
       <c r="BF130" s="22"/>
       <c r="BG130" s="22"/>
@@ -14760,6 +14897,7 @@
     <row r="131" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
+      <c r="G131" s="40"/>
       <c r="BE131" s="22"/>
       <c r="BF131" s="22"/>
       <c r="BG131" s="22"/>
@@ -14864,6 +15002,7 @@
     <row r="132" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B132" s="19"/>
       <c r="C132" s="19"/>
+      <c r="G132" s="40"/>
       <c r="BE132" s="22"/>
       <c r="BF132" s="22"/>
       <c r="BG132" s="22"/>
@@ -14968,6 +15107,7 @@
     <row r="133" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
+      <c r="G133" s="40"/>
       <c r="BE133" s="22"/>
       <c r="BF133" s="22"/>
       <c r="BG133" s="22"/>
@@ -15072,6 +15212,7 @@
     <row r="134" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
+      <c r="G134" s="40"/>
       <c r="BE134" s="22"/>
       <c r="BF134" s="22"/>
       <c r="BG134" s="22"/>
@@ -15176,6 +15317,7 @@
     <row r="135" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B135" s="19"/>
       <c r="C135" s="19"/>
+      <c r="G135" s="40"/>
       <c r="BE135" s="22"/>
       <c r="BF135" s="22"/>
       <c r="BG135" s="22"/>
@@ -15280,6 +15422,7 @@
     <row r="136" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136" s="19"/>
       <c r="C136" s="19"/>
+      <c r="G136" s="40"/>
       <c r="BE136" s="22"/>
       <c r="BF136" s="22"/>
       <c r="BG136" s="22"/>
@@ -15384,6 +15527,7 @@
     <row r="137" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B137" s="19"/>
       <c r="C137" s="19"/>
+      <c r="G137" s="40"/>
       <c r="BE137" s="22"/>
       <c r="BF137" s="22"/>
       <c r="BG137" s="22"/>
@@ -15488,6 +15632,7 @@
     <row r="138" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B138" s="19"/>
       <c r="C138" s="19"/>
+      <c r="G138" s="40"/>
       <c r="BE138" s="22"/>
       <c r="BF138" s="22"/>
       <c r="BG138" s="22"/>
@@ -15592,6 +15737,7 @@
     <row r="139" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B139" s="19"/>
       <c r="C139" s="19"/>
+      <c r="G139" s="40"/>
       <c r="BE139" s="22"/>
       <c r="BF139" s="22"/>
       <c r="BG139" s="22"/>
@@ -15696,6 +15842,7 @@
     <row r="140" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B140" s="19"/>
       <c r="C140" s="19"/>
+      <c r="G140" s="40"/>
       <c r="BE140" s="22"/>
       <c r="BF140" s="22"/>
       <c r="BG140" s="22"/>
@@ -15800,6 +15947,7 @@
     <row r="141" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B141" s="19"/>
       <c r="C141" s="19"/>
+      <c r="G141" s="40"/>
       <c r="BE141" s="22"/>
       <c r="BF141" s="22"/>
       <c r="BG141" s="22"/>
@@ -15904,6 +16052,7 @@
     <row r="142" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B142" s="19"/>
       <c r="C142" s="19"/>
+      <c r="G142" s="40"/>
       <c r="BE142" s="22"/>
       <c r="BF142" s="22"/>
       <c r="BG142" s="22"/>
@@ -16008,6 +16157,7 @@
     <row r="143" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B143" s="19"/>
       <c r="C143" s="19"/>
+      <c r="G143" s="40"/>
       <c r="BE143" s="22"/>
       <c r="BF143" s="22"/>
       <c r="BG143" s="22"/>
@@ -16112,6 +16262,7 @@
     <row r="144" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B144" s="19"/>
       <c r="C144" s="19"/>
+      <c r="G144" s="40"/>
       <c r="BE144" s="22"/>
       <c r="BF144" s="22"/>
       <c r="BG144" s="22"/>
@@ -16216,6 +16367,7 @@
     <row r="145" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B145" s="19"/>
       <c r="C145" s="19"/>
+      <c r="G145" s="40"/>
       <c r="BE145" s="22"/>
       <c r="BF145" s="22"/>
       <c r="BG145" s="22"/>
@@ -16320,6 +16472,7 @@
     <row r="146" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B146" s="19"/>
       <c r="C146" s="19"/>
+      <c r="G146" s="40"/>
       <c r="BE146" s="22"/>
       <c r="BF146" s="22"/>
       <c r="BG146" s="22"/>
@@ -16424,6 +16577,7 @@
     <row r="147" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147" s="19"/>
       <c r="C147" s="19"/>
+      <c r="G147" s="40"/>
       <c r="BE147" s="22"/>
       <c r="BF147" s="22"/>
       <c r="BG147" s="22"/>
@@ -16528,6 +16682,7 @@
     <row r="148" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B148" s="19"/>
       <c r="C148" s="19"/>
+      <c r="G148" s="40"/>
       <c r="BE148" s="22"/>
       <c r="BF148" s="22"/>
       <c r="BG148" s="22"/>
@@ -16632,6 +16787,7 @@
     <row r="149" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B149" s="19"/>
       <c r="C149" s="19"/>
+      <c r="G149" s="40"/>
       <c r="BE149" s="22"/>
       <c r="BF149" s="22"/>
       <c r="BG149" s="22"/>
@@ -16736,6 +16892,7 @@
     <row r="150" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B150" s="19"/>
       <c r="C150" s="19"/>
+      <c r="G150" s="40"/>
       <c r="BE150" s="22"/>
       <c r="BF150" s="22"/>
       <c r="BG150" s="22"/>
@@ -16840,6 +16997,7 @@
     <row r="151" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B151" s="19"/>
       <c r="C151" s="19"/>
+      <c r="G151" s="40"/>
       <c r="BE151" s="22"/>
       <c r="BF151" s="22"/>
       <c r="BG151" s="22"/>
@@ -16944,6 +17102,7 @@
     <row r="152" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B152" s="19"/>
       <c r="C152" s="19"/>
+      <c r="G152" s="40"/>
       <c r="BE152" s="22"/>
       <c r="BF152" s="22"/>
       <c r="BG152" s="22"/>
@@ -17048,6 +17207,7 @@
     <row r="153" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B153" s="19"/>
       <c r="C153" s="19"/>
+      <c r="G153" s="40"/>
       <c r="BE153" s="22"/>
       <c r="BF153" s="22"/>
       <c r="BG153" s="22"/>
@@ -17152,6 +17312,7 @@
     <row r="154" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B154" s="19"/>
       <c r="C154" s="19"/>
+      <c r="G154" s="40"/>
       <c r="BE154" s="22"/>
       <c r="BF154" s="22"/>
       <c r="BG154" s="22"/>
@@ -17256,6 +17417,7 @@
     <row r="155" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B155" s="19"/>
       <c r="C155" s="19"/>
+      <c r="G155" s="40"/>
       <c r="BE155" s="22"/>
       <c r="BF155" s="22"/>
       <c r="BG155" s="22"/>
@@ -17360,6 +17522,7 @@
     <row r="156" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B156" s="19"/>
       <c r="C156" s="19"/>
+      <c r="G156" s="40"/>
       <c r="BE156" s="22"/>
       <c r="BF156" s="22"/>
       <c r="BG156" s="22"/>
@@ -17464,6 +17627,7 @@
     <row r="157" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B157" s="19"/>
       <c r="C157" s="19"/>
+      <c r="G157" s="40"/>
       <c r="BE157" s="22"/>
       <c r="BF157" s="22"/>
       <c r="BG157" s="22"/>
@@ -17568,6 +17732,7 @@
     <row r="158" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B158" s="19"/>
       <c r="C158" s="19"/>
+      <c r="G158" s="40"/>
       <c r="BE158" s="22"/>
       <c r="BF158" s="22"/>
       <c r="BG158" s="22"/>
@@ -17672,6 +17837,7 @@
     <row r="159" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B159" s="19"/>
       <c r="C159" s="19"/>
+      <c r="G159" s="40"/>
       <c r="BE159" s="22"/>
       <c r="BF159" s="22"/>
       <c r="BG159" s="22"/>
@@ -17776,6 +17942,7 @@
     <row r="160" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B160" s="19"/>
       <c r="C160" s="19"/>
+      <c r="G160" s="40"/>
       <c r="BE160" s="22"/>
       <c r="BF160" s="22"/>
       <c r="BG160" s="22"/>
@@ -17880,6 +18047,7 @@
     <row r="161" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B161" s="19"/>
       <c r="C161" s="19"/>
+      <c r="G161" s="40"/>
       <c r="BE161" s="22"/>
       <c r="BF161" s="22"/>
       <c r="BG161" s="22"/>
@@ -17984,6 +18152,7 @@
     <row r="162" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="19"/>
       <c r="C162" s="19"/>
+      <c r="G162" s="40"/>
       <c r="BE162" s="22"/>
       <c r="BF162" s="22"/>
       <c r="BG162" s="22"/>
@@ -18088,6 +18257,7 @@
     <row r="163" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B163" s="19"/>
       <c r="C163" s="19"/>
+      <c r="G163" s="40"/>
       <c r="BE163" s="22"/>
       <c r="BF163" s="22"/>
       <c r="BG163" s="22"/>
@@ -18192,6 +18362,7 @@
     <row r="164" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B164" s="19"/>
       <c r="C164" s="19"/>
+      <c r="G164" s="40"/>
       <c r="BE164" s="22"/>
       <c r="BF164" s="22"/>
       <c r="BG164" s="22"/>
@@ -18296,6 +18467,7 @@
     <row r="165" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="19"/>
       <c r="C165" s="19"/>
+      <c r="G165" s="40"/>
       <c r="BE165" s="22"/>
       <c r="BF165" s="22"/>
       <c r="BG165" s="22"/>
@@ -18400,6 +18572,7 @@
     <row r="166" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="19"/>
       <c r="C166" s="19"/>
+      <c r="G166" s="40"/>
       <c r="BE166" s="22"/>
       <c r="BF166" s="22"/>
       <c r="BG166" s="22"/>
@@ -18504,6 +18677,7 @@
     <row r="167" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="19"/>
       <c r="C167" s="19"/>
+      <c r="G167" s="40"/>
       <c r="BE167" s="22"/>
       <c r="BF167" s="22"/>
       <c r="BG167" s="22"/>
@@ -18608,6 +18782,7 @@
     <row r="168" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="19"/>
       <c r="C168" s="19"/>
+      <c r="G168" s="40"/>
       <c r="BE168" s="22"/>
       <c r="BF168" s="22"/>
       <c r="BG168" s="22"/>
@@ -18712,6 +18887,7 @@
     <row r="169" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B169" s="19"/>
       <c r="C169" s="19"/>
+      <c r="G169" s="40"/>
       <c r="BE169" s="22"/>
       <c r="BF169" s="22"/>
       <c r="BG169" s="22"/>
@@ -18816,6 +18992,7 @@
     <row r="170" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B170" s="19"/>
       <c r="C170" s="19"/>
+      <c r="G170" s="40"/>
       <c r="BE170" s="22"/>
       <c r="BF170" s="22"/>
       <c r="BG170" s="22"/>
@@ -18920,6 +19097,7 @@
     <row r="171" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B171" s="19"/>
       <c r="C171" s="19"/>
+      <c r="G171" s="40"/>
       <c r="BE171" s="22"/>
       <c r="BF171" s="22"/>
       <c r="BG171" s="22"/>
@@ -19024,6 +19202,7 @@
     <row r="172" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B172" s="19"/>
       <c r="C172" s="19"/>
+      <c r="G172" s="40"/>
       <c r="BE172" s="22"/>
       <c r="BF172" s="22"/>
       <c r="BG172" s="22"/>
@@ -19128,6 +19307,7 @@
     <row r="173" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B173" s="19"/>
       <c r="C173" s="19"/>
+      <c r="G173" s="40"/>
       <c r="BE173" s="22"/>
       <c r="BF173" s="22"/>
       <c r="BG173" s="22"/>
@@ -19232,6 +19412,7 @@
     <row r="174" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="19"/>
       <c r="C174" s="19"/>
+      <c r="G174" s="40"/>
       <c r="BE174" s="22"/>
       <c r="BF174" s="22"/>
       <c r="BG174" s="22"/>
@@ -19336,6 +19517,7 @@
     <row r="175" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="19"/>
       <c r="C175" s="19"/>
+      <c r="G175" s="40"/>
       <c r="BE175" s="22"/>
       <c r="BF175" s="22"/>
       <c r="BG175" s="22"/>
@@ -19440,6 +19622,7 @@
     <row r="176" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="19"/>
       <c r="C176" s="19"/>
+      <c r="G176" s="40"/>
       <c r="BE176" s="22"/>
       <c r="BF176" s="22"/>
       <c r="BG176" s="22"/>
@@ -19544,6 +19727,7 @@
     <row r="177" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B177" s="19"/>
       <c r="C177" s="19"/>
+      <c r="G177" s="40"/>
       <c r="BE177" s="22"/>
       <c r="BF177" s="22"/>
       <c r="BG177" s="22"/>
@@ -19648,6 +19832,7 @@
     <row r="178" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B178" s="19"/>
       <c r="C178" s="19"/>
+      <c r="G178" s="40"/>
       <c r="BE178" s="22"/>
       <c r="BF178" s="22"/>
       <c r="BG178" s="22"/>
@@ -19752,6 +19937,7 @@
     <row r="179" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B179" s="19"/>
       <c r="C179" s="19"/>
+      <c r="G179" s="40"/>
       <c r="BE179" s="22"/>
       <c r="BF179" s="22"/>
       <c r="BG179" s="22"/>
@@ -19856,6 +20042,7 @@
     <row r="180" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B180" s="19"/>
       <c r="C180" s="19"/>
+      <c r="G180" s="40"/>
       <c r="BE180" s="22"/>
       <c r="BF180" s="22"/>
       <c r="BG180" s="22"/>
@@ -19960,6 +20147,7 @@
     <row r="181" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B181" s="19"/>
       <c r="C181" s="19"/>
+      <c r="G181" s="40"/>
       <c r="BE181" s="22"/>
       <c r="BF181" s="22"/>
       <c r="BG181" s="22"/>
@@ -20064,6 +20252,7 @@
     <row r="182" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B182" s="19"/>
       <c r="C182" s="19"/>
+      <c r="G182" s="40"/>
       <c r="BE182" s="22"/>
       <c r="BF182" s="22"/>
       <c r="BG182" s="22"/>
@@ -20168,6 +20357,7 @@
     <row r="183" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" s="19"/>
       <c r="C183" s="19"/>
+      <c r="G183" s="40"/>
       <c r="BE183" s="22"/>
       <c r="BF183" s="22"/>
       <c r="BG183" s="22"/>
@@ -20272,6 +20462,7 @@
     <row r="184" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" s="19"/>
       <c r="C184" s="19"/>
+      <c r="G184" s="40"/>
       <c r="BE184" s="22"/>
       <c r="BF184" s="22"/>
       <c r="BG184" s="22"/>
@@ -20376,6 +20567,7 @@
     <row r="185" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B185" s="19"/>
       <c r="C185" s="19"/>
+      <c r="G185" s="40"/>
       <c r="BE185" s="22"/>
       <c r="BF185" s="22"/>
       <c r="BG185" s="22"/>
@@ -20480,6 +20672,7 @@
     <row r="186" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B186" s="19"/>
       <c r="C186" s="19"/>
+      <c r="G186" s="40"/>
       <c r="BE186" s="22"/>
       <c r="BF186" s="22"/>
       <c r="BG186" s="22"/>
@@ -20584,6 +20777,7 @@
     <row r="187" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B187" s="19"/>
       <c r="C187" s="19"/>
+      <c r="G187" s="40"/>
       <c r="BE187" s="22"/>
       <c r="BF187" s="22"/>
       <c r="BG187" s="22"/>
@@ -20688,6 +20882,7 @@
     <row r="188" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B188" s="19"/>
       <c r="C188" s="19"/>
+      <c r="G188" s="40"/>
       <c r="BE188" s="22"/>
       <c r="BF188" s="22"/>
       <c r="BG188" s="22"/>
@@ -20792,6 +20987,7 @@
     <row r="189" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B189" s="19"/>
       <c r="C189" s="19"/>
+      <c r="G189" s="40"/>
       <c r="BE189" s="22"/>
       <c r="BF189" s="22"/>
       <c r="BG189" s="22"/>
@@ -20896,6 +21092,7 @@
     <row r="190" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B190" s="19"/>
       <c r="C190" s="19"/>
+      <c r="G190" s="40"/>
       <c r="BE190" s="22"/>
       <c r="BF190" s="22"/>
       <c r="BG190" s="22"/>
@@ -21000,6 +21197,7 @@
     <row r="191" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B191" s="19"/>
       <c r="C191" s="19"/>
+      <c r="G191" s="40"/>
       <c r="BE191" s="22"/>
       <c r="BF191" s="22"/>
       <c r="BG191" s="22"/>
@@ -21104,6 +21302,7 @@
     <row r="192" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B192" s="19"/>
       <c r="C192" s="19"/>
+      <c r="G192" s="40"/>
       <c r="BE192" s="22"/>
       <c r="BF192" s="22"/>
       <c r="BG192" s="22"/>
@@ -21208,6 +21407,7 @@
     <row r="193" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B193" s="19"/>
       <c r="C193" s="19"/>
+      <c r="G193" s="40"/>
       <c r="BE193" s="22"/>
       <c r="BF193" s="22"/>
       <c r="BG193" s="22"/>
@@ -21312,6 +21512,7 @@
     <row r="194" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B194" s="19"/>
       <c r="C194" s="19"/>
+      <c r="G194" s="40"/>
       <c r="BE194" s="22"/>
       <c r="BF194" s="22"/>
       <c r="BG194" s="22"/>
@@ -21416,6 +21617,7 @@
     <row r="195" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B195" s="19"/>
       <c r="C195" s="19"/>
+      <c r="G195" s="40"/>
       <c r="BE195" s="22"/>
       <c r="BF195" s="22"/>
       <c r="BG195" s="22"/>
@@ -21520,6 +21722,7 @@
     <row r="196" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B196" s="19"/>
       <c r="C196" s="19"/>
+      <c r="G196" s="40"/>
       <c r="BE196" s="22"/>
       <c r="BF196" s="22"/>
       <c r="BG196" s="22"/>
@@ -21624,6 +21827,7 @@
     <row r="197" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B197" s="19"/>
       <c r="C197" s="19"/>
+      <c r="G197" s="40"/>
       <c r="BE197" s="22"/>
       <c r="BF197" s="22"/>
       <c r="BG197" s="22"/>
@@ -21728,6 +21932,7 @@
     <row r="198" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B198" s="19"/>
       <c r="C198" s="19"/>
+      <c r="G198" s="40"/>
       <c r="BE198" s="22"/>
       <c r="BF198" s="22"/>
       <c r="BG198" s="22"/>
@@ -21832,6 +22037,7 @@
     <row r="199" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B199" s="19"/>
       <c r="C199" s="19"/>
+      <c r="G199" s="40"/>
       <c r="BE199" s="22"/>
       <c r="BF199" s="22"/>
       <c r="BG199" s="22"/>
@@ -21936,6 +22142,7 @@
     <row r="200" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B200" s="19"/>
       <c r="C200" s="19"/>
+      <c r="G200" s="40"/>
       <c r="BE200" s="22"/>
       <c r="BF200" s="22"/>
       <c r="BG200" s="22"/>
@@ -22040,6 +22247,7 @@
     <row r="201" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B201" s="19"/>
       <c r="C201" s="19"/>
+      <c r="G201" s="40"/>
       <c r="BE201" s="22"/>
       <c r="BF201" s="22"/>
       <c r="BG201" s="22"/>
@@ -22144,6 +22352,7 @@
     <row r="202" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B202" s="19"/>
       <c r="C202" s="19"/>
+      <c r="G202" s="40"/>
       <c r="BE202" s="22"/>
       <c r="BF202" s="22"/>
       <c r="BG202" s="22"/>
@@ -22248,6 +22457,7 @@
     <row r="203" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B203" s="19"/>
       <c r="C203" s="19"/>
+      <c r="G203" s="40"/>
       <c r="BE203" s="22"/>
       <c r="BF203" s="22"/>
       <c r="BG203" s="22"/>
@@ -22352,6 +22562,7 @@
     <row r="204" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B204" s="19"/>
       <c r="C204" s="19"/>
+      <c r="G204" s="40"/>
       <c r="BE204" s="22"/>
       <c r="BF204" s="22"/>
       <c r="BG204" s="22"/>
@@ -22456,6 +22667,7 @@
     <row r="205" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B205" s="19"/>
       <c r="C205" s="19"/>
+      <c r="G205" s="40"/>
       <c r="BE205" s="22"/>
       <c r="BF205" s="22"/>
       <c r="BG205" s="22"/>
@@ -22560,6 +22772,7 @@
     <row r="206" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B206" s="19"/>
       <c r="C206" s="19"/>
+      <c r="G206" s="40"/>
       <c r="BE206" s="22"/>
       <c r="BF206" s="22"/>
       <c r="BG206" s="22"/>
@@ -22664,6 +22877,7 @@
     <row r="207" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B207" s="19"/>
       <c r="C207" s="19"/>
+      <c r="G207" s="40"/>
       <c r="BE207" s="22"/>
       <c r="BF207" s="22"/>
       <c r="BG207" s="22"/>
@@ -22768,6 +22982,7 @@
     <row r="208" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B208" s="19"/>
       <c r="C208" s="19"/>
+      <c r="G208" s="40"/>
       <c r="BE208" s="22"/>
       <c r="BF208" s="22"/>
       <c r="BG208" s="22"/>
@@ -22872,6 +23087,7 @@
     <row r="209" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B209" s="19"/>
       <c r="C209" s="19"/>
+      <c r="G209" s="40"/>
       <c r="BE209" s="22"/>
       <c r="BF209" s="22"/>
       <c r="BG209" s="22"/>
@@ -22976,6 +23192,7 @@
     <row r="210" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B210" s="19"/>
       <c r="C210" s="19"/>
+      <c r="G210" s="40"/>
       <c r="BE210" s="22"/>
       <c r="BF210" s="22"/>
       <c r="BG210" s="22"/>
@@ -23080,6 +23297,7 @@
     <row r="211" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B211" s="19"/>
       <c r="C211" s="19"/>
+      <c r="G211" s="40"/>
       <c r="BE211" s="22"/>
       <c r="BF211" s="22"/>
       <c r="BG211" s="22"/>
@@ -23184,6 +23402,7 @@
     <row r="212" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B212" s="19"/>
       <c r="C212" s="19"/>
+      <c r="G212" s="40"/>
       <c r="BE212" s="22"/>
       <c r="BF212" s="22"/>
       <c r="BG212" s="22"/>
@@ -23288,6 +23507,7 @@
     <row r="213" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B213" s="19"/>
       <c r="C213" s="19"/>
+      <c r="G213" s="40"/>
       <c r="BE213" s="22"/>
       <c r="BF213" s="22"/>
       <c r="BG213" s="22"/>
@@ -23392,6 +23612,7 @@
     <row r="214" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B214" s="19"/>
       <c r="C214" s="19"/>
+      <c r="G214" s="40"/>
       <c r="BE214" s="22"/>
       <c r="BF214" s="22"/>
       <c r="BG214" s="22"/>
@@ -23496,6 +23717,7 @@
     <row r="215" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B215" s="19"/>
       <c r="C215" s="19"/>
+      <c r="G215" s="40"/>
       <c r="BE215" s="22"/>
       <c r="BF215" s="22"/>
       <c r="BG215" s="22"/>
@@ -23600,6 +23822,7 @@
     <row r="216" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B216" s="19"/>
       <c r="C216" s="19"/>
+      <c r="G216" s="40"/>
       <c r="BE216" s="22"/>
       <c r="BF216" s="22"/>
       <c r="BG216" s="22"/>
@@ -23704,6 +23927,7 @@
     <row r="217" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B217" s="19"/>
       <c r="C217" s="19"/>
+      <c r="G217" s="40"/>
       <c r="BE217" s="22"/>
       <c r="BF217" s="22"/>
       <c r="BG217" s="22"/>
@@ -23808,6 +24032,7 @@
     <row r="218" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B218" s="19"/>
       <c r="C218" s="19"/>
+      <c r="G218" s="40"/>
       <c r="BE218" s="22"/>
       <c r="BF218" s="22"/>
       <c r="BG218" s="22"/>
@@ -23912,6 +24137,7 @@
     <row r="219" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B219" s="19"/>
       <c r="C219" s="19"/>
+      <c r="G219" s="40"/>
       <c r="BE219" s="22"/>
       <c r="BF219" s="22"/>
       <c r="BG219" s="22"/>
@@ -24016,6 +24242,7 @@
     <row r="220" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B220" s="19"/>
       <c r="C220" s="19"/>
+      <c r="G220" s="40"/>
       <c r="BE220" s="22"/>
       <c r="BF220" s="22"/>
       <c r="BG220" s="22"/>
@@ -24120,6 +24347,7 @@
     <row r="221" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B221" s="19"/>
       <c r="C221" s="19"/>
+      <c r="G221" s="40"/>
       <c r="BE221" s="22"/>
       <c r="BF221" s="22"/>
       <c r="BG221" s="22"/>
@@ -24224,6 +24452,7 @@
     <row r="222" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B222" s="19"/>
       <c r="C222" s="19"/>
+      <c r="G222" s="40"/>
       <c r="BE222" s="22"/>
       <c r="BF222" s="22"/>
       <c r="BG222" s="22"/>
@@ -24328,6 +24557,7 @@
     <row r="223" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B223" s="19"/>
       <c r="C223" s="19"/>
+      <c r="G223" s="40"/>
       <c r="BE223" s="22"/>
       <c r="BF223" s="22"/>
       <c r="BG223" s="22"/>
@@ -24432,6 +24662,7 @@
     <row r="224" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B224" s="19"/>
       <c r="C224" s="19"/>
+      <c r="G224" s="40"/>
       <c r="BE224" s="22"/>
       <c r="BF224" s="22"/>
       <c r="BG224" s="22"/>
@@ -24536,6 +24767,7 @@
     <row r="225" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B225" s="19"/>
       <c r="C225" s="19"/>
+      <c r="G225" s="40"/>
       <c r="BE225" s="22"/>
       <c r="BF225" s="22"/>
       <c r="BG225" s="22"/>
@@ -24640,6 +24872,7 @@
     <row r="226" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B226" s="19"/>
       <c r="C226" s="19"/>
+      <c r="G226" s="40"/>
       <c r="BE226" s="22"/>
       <c r="BF226" s="22"/>
       <c r="BG226" s="22"/>
@@ -24744,6 +24977,7 @@
     <row r="227" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B227" s="19"/>
       <c r="C227" s="19"/>
+      <c r="G227" s="40"/>
       <c r="BE227" s="22"/>
       <c r="BF227" s="22"/>
       <c r="BG227" s="22"/>
@@ -24848,6 +25082,7 @@
     <row r="228" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B228" s="19"/>
       <c r="C228" s="19"/>
+      <c r="G228" s="40"/>
       <c r="BE228" s="22"/>
       <c r="BF228" s="22"/>
       <c r="BG228" s="22"/>
@@ -24952,6 +25187,7 @@
     <row r="229" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B229" s="19"/>
       <c r="C229" s="19"/>
+      <c r="G229" s="40"/>
       <c r="BE229" s="22"/>
       <c r="BF229" s="22"/>
       <c r="BG229" s="22"/>
@@ -25056,6 +25292,7 @@
     <row r="230" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B230" s="19"/>
       <c r="C230" s="19"/>
+      <c r="G230" s="40"/>
       <c r="BE230" s="22"/>
       <c r="BF230" s="22"/>
       <c r="BG230" s="22"/>
@@ -25160,6 +25397,7 @@
     <row r="231" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B231" s="19"/>
       <c r="C231" s="19"/>
+      <c r="G231" s="40"/>
       <c r="BE231" s="22"/>
       <c r="BF231" s="22"/>
       <c r="BG231" s="22"/>
@@ -25264,6 +25502,7 @@
     <row r="232" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B232" s="19"/>
       <c r="C232" s="19"/>
+      <c r="G232" s="40"/>
       <c r="BE232" s="22"/>
       <c r="BF232" s="22"/>
       <c r="BG232" s="22"/>
@@ -25368,6 +25607,7 @@
     <row r="233" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B233" s="19"/>
       <c r="C233" s="19"/>
+      <c r="G233" s="40"/>
       <c r="BE233" s="22"/>
       <c r="BF233" s="22"/>
       <c r="BG233" s="22"/>
@@ -25472,6 +25712,7 @@
     <row r="234" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B234" s="19"/>
       <c r="C234" s="19"/>
+      <c r="G234" s="40"/>
       <c r="BE234" s="22"/>
       <c r="BF234" s="22"/>
       <c r="BG234" s="22"/>
@@ -25576,6 +25817,7 @@
     <row r="235" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B235" s="19"/>
       <c r="C235" s="19"/>
+      <c r="G235" s="40"/>
       <c r="BE235" s="22"/>
       <c r="BF235" s="22"/>
       <c r="BG235" s="22"/>
@@ -25680,6 +25922,7 @@
     <row r="236" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B236" s="19"/>
       <c r="C236" s="19"/>
+      <c r="G236" s="40"/>
       <c r="BE236" s="22"/>
       <c r="BF236" s="22"/>
       <c r="BG236" s="22"/>
@@ -25784,6 +26027,7 @@
     <row r="237" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B237" s="19"/>
       <c r="C237" s="19"/>
+      <c r="G237" s="40"/>
       <c r="BE237" s="22"/>
       <c r="BF237" s="22"/>
       <c r="BG237" s="22"/>
@@ -25888,6 +26132,7 @@
     <row r="238" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B238" s="19"/>
       <c r="C238" s="19"/>
+      <c r="G238" s="40"/>
       <c r="BE238" s="22"/>
       <c r="BF238" s="22"/>
       <c r="BG238" s="22"/>
@@ -25992,6 +26237,7 @@
     <row r="239" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B239" s="19"/>
       <c r="C239" s="19"/>
+      <c r="G239" s="40"/>
       <c r="BE239" s="22"/>
       <c r="BF239" s="22"/>
       <c r="BG239" s="22"/>
@@ -26096,6 +26342,7 @@
     <row r="240" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B240" s="19"/>
       <c r="C240" s="19"/>
+      <c r="G240" s="40"/>
       <c r="BE240" s="22"/>
       <c r="BF240" s="22"/>
       <c r="BG240" s="22"/>
@@ -26200,6 +26447,7 @@
     <row r="241" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B241" s="19"/>
       <c r="C241" s="19"/>
+      <c r="G241" s="40"/>
       <c r="BE241" s="22"/>
       <c r="BF241" s="22"/>
       <c r="BG241" s="22"/>
@@ -26304,6 +26552,7 @@
     <row r="242" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B242" s="19"/>
       <c r="C242" s="19"/>
+      <c r="G242" s="40"/>
       <c r="BE242" s="22"/>
       <c r="BF242" s="22"/>
       <c r="BG242" s="22"/>
@@ -26408,6 +26657,7 @@
     <row r="243" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B243" s="19"/>
       <c r="C243" s="19"/>
+      <c r="G243" s="40"/>
       <c r="BE243" s="22"/>
       <c r="BF243" s="22"/>
       <c r="BG243" s="22"/>
@@ -26512,6 +26762,7 @@
     <row r="244" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B244" s="19"/>
       <c r="C244" s="19"/>
+      <c r="G244" s="40"/>
       <c r="BE244" s="22"/>
       <c r="BF244" s="22"/>
       <c r="BG244" s="22"/>
@@ -26616,6 +26867,7 @@
     <row r="245" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B245" s="19"/>
       <c r="C245" s="19"/>
+      <c r="G245" s="40"/>
       <c r="BE245" s="22"/>
       <c r="BF245" s="22"/>
       <c r="BG245" s="22"/>
@@ -26720,6 +26972,7 @@
     <row r="246" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B246" s="19"/>
       <c r="C246" s="19"/>
+      <c r="G246" s="40"/>
       <c r="BE246" s="22"/>
       <c r="BF246" s="22"/>
       <c r="BG246" s="22"/>
@@ -26824,6 +27077,7 @@
     <row r="247" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B247" s="19"/>
       <c r="C247" s="19"/>
+      <c r="G247" s="40"/>
       <c r="BE247" s="22"/>
       <c r="BF247" s="22"/>
       <c r="BG247" s="22"/>
@@ -26928,6 +27182,7 @@
     <row r="248" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B248" s="19"/>
       <c r="C248" s="19"/>
+      <c r="G248" s="40"/>
       <c r="BE248" s="22"/>
       <c r="BF248" s="22"/>
       <c r="BG248" s="22"/>
@@ -27032,6 +27287,7 @@
     <row r="249" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B249" s="19"/>
       <c r="C249" s="19"/>
+      <c r="G249" s="40"/>
       <c r="BE249" s="22"/>
       <c r="BF249" s="22"/>
       <c r="BG249" s="22"/>
@@ -27136,6 +27392,7 @@
     <row r="250" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B250" s="19"/>
       <c r="C250" s="19"/>
+      <c r="G250" s="40"/>
       <c r="BE250" s="22"/>
       <c r="BF250" s="22"/>
       <c r="BG250" s="22"/>
@@ -27240,6 +27497,7 @@
     <row r="251" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B251" s="19"/>
       <c r="C251" s="19"/>
+      <c r="G251" s="40"/>
       <c r="BE251" s="22"/>
       <c r="BF251" s="22"/>
       <c r="BG251" s="22"/>
@@ -27344,6 +27602,7 @@
     <row r="252" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B252" s="19"/>
       <c r="C252" s="19"/>
+      <c r="G252" s="40"/>
       <c r="BE252" s="22"/>
       <c r="BF252" s="22"/>
       <c r="BG252" s="22"/>
@@ -27448,6 +27707,7 @@
     <row r="253" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B253" s="19"/>
       <c r="C253" s="19"/>
+      <c r="G253" s="40"/>
       <c r="BE253" s="22"/>
       <c r="BF253" s="22"/>
       <c r="BG253" s="22"/>
@@ -27552,6 +27812,7 @@
     <row r="254" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B254" s="19"/>
       <c r="C254" s="19"/>
+      <c r="G254" s="40"/>
       <c r="BE254" s="22"/>
       <c r="BF254" s="22"/>
       <c r="BG254" s="22"/>
@@ -27656,6 +27917,7 @@
     <row r="255" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B255" s="19"/>
       <c r="C255" s="19"/>
+      <c r="G255" s="40"/>
       <c r="BE255" s="22"/>
       <c r="BF255" s="22"/>
       <c r="BG255" s="22"/>
@@ -27760,6 +28022,7 @@
     <row r="256" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B256" s="19"/>
       <c r="C256" s="19"/>
+      <c r="G256" s="40"/>
       <c r="BE256" s="22"/>
       <c r="BF256" s="22"/>
       <c r="BG256" s="22"/>
@@ -27864,6 +28127,7 @@
     <row r="257" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B257" s="19"/>
       <c r="C257" s="19"/>
+      <c r="G257" s="40"/>
       <c r="BE257" s="22"/>
       <c r="BF257" s="22"/>
       <c r="BG257" s="22"/>
@@ -27968,6 +28232,7 @@
     <row r="258" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B258" s="19"/>
       <c r="C258" s="19"/>
+      <c r="G258" s="40"/>
       <c r="BE258" s="22"/>
       <c r="BF258" s="22"/>
       <c r="BG258" s="22"/>
@@ -28072,6 +28337,7 @@
     <row r="259" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B259" s="19"/>
       <c r="C259" s="19"/>
+      <c r="G259" s="40"/>
       <c r="BE259" s="22"/>
       <c r="BF259" s="22"/>
       <c r="BG259" s="22"/>
@@ -28176,6 +28442,7 @@
     <row r="260" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B260" s="19"/>
       <c r="C260" s="19"/>
+      <c r="G260" s="40"/>
       <c r="BE260" s="22"/>
       <c r="BF260" s="22"/>
       <c r="BG260" s="22"/>
@@ -28280,6 +28547,7 @@
     <row r="261" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B261" s="19"/>
       <c r="C261" s="19"/>
+      <c r="G261" s="40"/>
       <c r="BE261" s="22"/>
       <c r="BF261" s="22"/>
       <c r="BG261" s="22"/>
@@ -28384,6 +28652,7 @@
     <row r="262" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B262" s="19"/>
       <c r="C262" s="19"/>
+      <c r="G262" s="40"/>
       <c r="BE262" s="22"/>
       <c r="BF262" s="22"/>
       <c r="BG262" s="22"/>
@@ -28488,6 +28757,7 @@
     <row r="263" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B263" s="19"/>
       <c r="C263" s="19"/>
+      <c r="G263" s="40"/>
       <c r="BE263" s="22"/>
       <c r="BF263" s="22"/>
       <c r="BG263" s="22"/>
@@ -28592,6 +28862,7 @@
     <row r="264" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B264" s="19"/>
       <c r="C264" s="19"/>
+      <c r="G264" s="40"/>
       <c r="BE264" s="22"/>
       <c r="BF264" s="22"/>
       <c r="BG264" s="22"/>
@@ -28696,6 +28967,7 @@
     <row r="265" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B265" s="19"/>
       <c r="C265" s="19"/>
+      <c r="G265" s="40"/>
       <c r="BE265" s="22"/>
       <c r="BF265" s="22"/>
       <c r="BG265" s="22"/>
@@ -28800,6 +29072,7 @@
     <row r="266" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B266" s="19"/>
       <c r="C266" s="19"/>
+      <c r="G266" s="40"/>
       <c r="BE266" s="22"/>
       <c r="BF266" s="22"/>
       <c r="BG266" s="22"/>
@@ -28904,6 +29177,7 @@
     <row r="267" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B267" s="19"/>
       <c r="C267" s="19"/>
+      <c r="G267" s="40"/>
       <c r="BE267" s="22"/>
       <c r="BF267" s="22"/>
       <c r="BG267" s="22"/>
@@ -29008,6 +29282,7 @@
     <row r="268" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B268" s="19"/>
       <c r="C268" s="19"/>
+      <c r="G268" s="40"/>
       <c r="BE268" s="22"/>
       <c r="BF268" s="22"/>
       <c r="BG268" s="22"/>
@@ -29112,6 +29387,7 @@
     <row r="269" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B269" s="19"/>
       <c r="C269" s="19"/>
+      <c r="G269" s="40"/>
       <c r="BE269" s="22"/>
       <c r="BF269" s="22"/>
       <c r="BG269" s="22"/>
@@ -29216,6 +29492,7 @@
     <row r="270" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B270" s="19"/>
       <c r="C270" s="19"/>
+      <c r="G270" s="40"/>
       <c r="BE270" s="22"/>
       <c r="BF270" s="22"/>
       <c r="BG270" s="22"/>
@@ -29320,6 +29597,7 @@
     <row r="271" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B271" s="19"/>
       <c r="C271" s="19"/>
+      <c r="G271" s="40"/>
       <c r="BE271" s="22"/>
       <c r="BF271" s="22"/>
       <c r="BG271" s="22"/>
@@ -29424,6 +29702,7 @@
     <row r="272" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B272" s="19"/>
       <c r="C272" s="19"/>
+      <c r="G272" s="40"/>
       <c r="BE272" s="22"/>
       <c r="BF272" s="22"/>
       <c r="BG272" s="22"/>
@@ -29528,6 +29807,7 @@
     <row r="273" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B273" s="19"/>
       <c r="C273" s="19"/>
+      <c r="G273" s="40"/>
       <c r="BE273" s="22"/>
       <c r="BF273" s="22"/>
       <c r="BG273" s="22"/>
@@ -29632,6 +29912,7 @@
     <row r="274" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B274" s="19"/>
       <c r="C274" s="19"/>
+      <c r="G274" s="40"/>
       <c r="BE274" s="22"/>
       <c r="BF274" s="22"/>
       <c r="BG274" s="22"/>
@@ -29736,6 +30017,7 @@
     <row r="275" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B275" s="19"/>
       <c r="C275" s="19"/>
+      <c r="G275" s="40"/>
       <c r="BE275" s="22"/>
       <c r="BF275" s="22"/>
       <c r="BG275" s="22"/>
@@ -29840,6 +30122,7 @@
     <row r="276" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B276" s="19"/>
       <c r="C276" s="19"/>
+      <c r="G276" s="40"/>
       <c r="BE276" s="22"/>
       <c r="BF276" s="22"/>
       <c r="BG276" s="22"/>
@@ -29944,6 +30227,7 @@
     <row r="277" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B277" s="19"/>
       <c r="C277" s="19"/>
+      <c r="G277" s="40"/>
       <c r="BE277" s="22"/>
       <c r="BF277" s="22"/>
       <c r="BG277" s="22"/>
@@ -30048,6 +30332,7 @@
     <row r="278" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B278" s="19"/>
       <c r="C278" s="19"/>
+      <c r="G278" s="40"/>
       <c r="BE278" s="22"/>
       <c r="BF278" s="22"/>
       <c r="BG278" s="22"/>
@@ -30152,6 +30437,7 @@
     <row r="279" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B279" s="19"/>
       <c r="C279" s="19"/>
+      <c r="G279" s="40"/>
       <c r="BE279" s="22"/>
       <c r="BF279" s="22"/>
       <c r="BG279" s="22"/>
@@ -30256,6 +30542,7 @@
     <row r="280" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B280" s="19"/>
       <c r="C280" s="19"/>
+      <c r="G280" s="40"/>
       <c r="BE280" s="22"/>
       <c r="BF280" s="22"/>
       <c r="BG280" s="22"/>
@@ -30360,6 +30647,7 @@
     <row r="281" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B281" s="19"/>
       <c r="C281" s="19"/>
+      <c r="G281" s="40"/>
       <c r="BE281" s="22"/>
       <c r="BF281" s="22"/>
       <c r="BG281" s="22"/>
@@ -30464,6 +30752,7 @@
     <row r="282" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B282" s="19"/>
       <c r="C282" s="19"/>
+      <c r="G282" s="40"/>
       <c r="BE282" s="22"/>
       <c r="BF282" s="22"/>
       <c r="BG282" s="22"/>
@@ -30568,6 +30857,7 @@
     <row r="283" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B283" s="19"/>
       <c r="C283" s="19"/>
+      <c r="G283" s="40"/>
       <c r="BE283" s="22"/>
       <c r="BF283" s="22"/>
       <c r="BG283" s="22"/>
@@ -30672,6 +30962,7 @@
     <row r="284" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B284" s="19"/>
       <c r="C284" s="19"/>
+      <c r="G284" s="40"/>
       <c r="BE284" s="22"/>
       <c r="BF284" s="22"/>
       <c r="BG284" s="22"/>
@@ -30776,6 +31067,7 @@
     <row r="285" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B285" s="19"/>
       <c r="C285" s="19"/>
+      <c r="G285" s="40"/>
       <c r="BE285" s="22"/>
       <c r="BF285" s="22"/>
       <c r="BG285" s="22"/>
@@ -30880,6 +31172,7 @@
     <row r="286" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B286" s="19"/>
       <c r="C286" s="19"/>
+      <c r="G286" s="40"/>
       <c r="BE286" s="22"/>
       <c r="BF286" s="22"/>
       <c r="BG286" s="22"/>
@@ -30984,6 +31277,7 @@
     <row r="287" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B287" s="19"/>
       <c r="C287" s="19"/>
+      <c r="G287" s="40"/>
       <c r="BE287" s="22"/>
       <c r="BF287" s="22"/>
       <c r="BG287" s="22"/>
@@ -31088,6 +31382,7 @@
     <row r="288" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B288" s="19"/>
       <c r="C288" s="19"/>
+      <c r="G288" s="40"/>
       <c r="BE288" s="22"/>
       <c r="BF288" s="22"/>
       <c r="BG288" s="22"/>
@@ -31192,6 +31487,7 @@
     <row r="289" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B289" s="19"/>
       <c r="C289" s="19"/>
+      <c r="G289" s="40"/>
       <c r="BE289" s="22"/>
       <c r="BF289" s="22"/>
       <c r="BG289" s="22"/>
@@ -31296,6 +31592,7 @@
     <row r="290" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B290" s="19"/>
       <c r="C290" s="19"/>
+      <c r="G290" s="40"/>
       <c r="BE290" s="22"/>
       <c r="BF290" s="22"/>
       <c r="BG290" s="22"/>
@@ -31400,6 +31697,7 @@
     <row r="291" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B291" s="19"/>
       <c r="C291" s="19"/>
+      <c r="G291" s="40"/>
       <c r="BE291" s="22"/>
       <c r="BF291" s="22"/>
       <c r="BG291" s="22"/>
@@ -31504,6 +31802,7 @@
     <row r="292" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B292" s="19"/>
       <c r="C292" s="19"/>
+      <c r="G292" s="40"/>
       <c r="BE292" s="22"/>
       <c r="BF292" s="22"/>
       <c r="BG292" s="22"/>
@@ -31608,6 +31907,7 @@
     <row r="293" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B293" s="19"/>
       <c r="C293" s="19"/>
+      <c r="G293" s="40"/>
       <c r="BE293" s="22"/>
       <c r="BF293" s="22"/>
       <c r="BG293" s="22"/>
@@ -31712,6 +32012,7 @@
     <row r="294" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B294" s="19"/>
       <c r="C294" s="19"/>
+      <c r="G294" s="40"/>
       <c r="BE294" s="22"/>
       <c r="BF294" s="22"/>
       <c r="BG294" s="22"/>
@@ -31816,6 +32117,7 @@
     <row r="295" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B295" s="19"/>
       <c r="C295" s="19"/>
+      <c r="G295" s="40"/>
       <c r="BE295" s="22"/>
       <c r="BF295" s="22"/>
       <c r="BG295" s="22"/>
@@ -31920,6 +32222,7 @@
     <row r="296" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B296" s="19"/>
       <c r="C296" s="19"/>
+      <c r="G296" s="40"/>
       <c r="BE296" s="22"/>
       <c r="BF296" s="22"/>
       <c r="BG296" s="22"/>
@@ -32024,6 +32327,7 @@
     <row r="297" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B297" s="19"/>
       <c r="C297" s="19"/>
+      <c r="G297" s="40"/>
       <c r="BE297" s="22"/>
       <c r="BF297" s="22"/>
       <c r="BG297" s="22"/>
@@ -32128,6 +32432,7 @@
     <row r="298" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B298" s="19"/>
       <c r="C298" s="19"/>
+      <c r="G298" s="40"/>
       <c r="BE298" s="22"/>
       <c r="BF298" s="22"/>
       <c r="BG298" s="22"/>
@@ -32232,6 +32537,7 @@
     <row r="299" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B299" s="19"/>
       <c r="C299" s="19"/>
+      <c r="G299" s="40"/>
       <c r="BE299" s="22"/>
       <c r="BF299" s="22"/>
       <c r="BG299" s="22"/>
@@ -32336,6 +32642,7 @@
     <row r="300" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B300" s="19"/>
       <c r="C300" s="19"/>
+      <c r="G300" s="40"/>
       <c r="BE300" s="22"/>
       <c r="BF300" s="22"/>
       <c r="BG300" s="22"/>
@@ -32440,6 +32747,7 @@
     <row r="301" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B301" s="19"/>
       <c r="C301" s="19"/>
+      <c r="G301" s="40"/>
       <c r="BE301" s="22"/>
       <c r="BF301" s="22"/>
       <c r="BG301" s="22"/>
@@ -32544,6 +32852,7 @@
     <row r="302" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B302" s="19"/>
       <c r="C302" s="19"/>
+      <c r="G302" s="40"/>
       <c r="BE302" s="22"/>
       <c r="BF302" s="22"/>
       <c r="BG302" s="22"/>
@@ -32648,6 +32957,7 @@
     <row r="303" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B303" s="19"/>
       <c r="C303" s="19"/>
+      <c r="G303" s="40"/>
       <c r="BE303" s="22"/>
       <c r="BF303" s="22"/>
       <c r="BG303" s="22"/>
@@ -32752,6 +33062,7 @@
     <row r="304" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B304" s="19"/>
       <c r="C304" s="19"/>
+      <c r="G304" s="40"/>
       <c r="BE304" s="22"/>
       <c r="BF304" s="22"/>
       <c r="BG304" s="22"/>
@@ -32856,6 +33167,7 @@
     <row r="305" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B305" s="19"/>
       <c r="C305" s="19"/>
+      <c r="G305" s="40"/>
       <c r="BE305" s="22"/>
       <c r="BF305" s="22"/>
       <c r="BG305" s="22"/>
@@ -32960,6 +33272,7 @@
     <row r="306" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B306" s="19"/>
       <c r="C306" s="19"/>
+      <c r="G306" s="40"/>
       <c r="BE306" s="22"/>
       <c r="BF306" s="22"/>
       <c r="BG306" s="22"/>
@@ -33064,6 +33377,7 @@
     <row r="307" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B307" s="19"/>
       <c r="C307" s="19"/>
+      <c r="G307" s="40"/>
       <c r="BE307" s="22"/>
       <c r="BF307" s="22"/>
       <c r="BG307" s="22"/>
@@ -33168,6 +33482,7 @@
     <row r="308" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B308" s="19"/>
       <c r="C308" s="19"/>
+      <c r="G308" s="40"/>
       <c r="BE308" s="22"/>
       <c r="BF308" s="22"/>
       <c r="BG308" s="22"/>
@@ -33272,6 +33587,7 @@
     <row r="309" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B309" s="19"/>
       <c r="C309" s="19"/>
+      <c r="G309" s="40"/>
       <c r="BE309" s="22"/>
       <c r="BF309" s="22"/>
       <c r="BG309" s="22"/>
@@ -33376,6 +33692,7 @@
     <row r="310" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B310" s="19"/>
       <c r="C310" s="19"/>
+      <c r="G310" s="40"/>
       <c r="BE310" s="22"/>
       <c r="BF310" s="22"/>
       <c r="BG310" s="22"/>
@@ -33480,6 +33797,7 @@
     <row r="311" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B311" s="19"/>
       <c r="C311" s="19"/>
+      <c r="G311" s="40"/>
       <c r="BE311" s="22"/>
       <c r="BF311" s="22"/>
       <c r="BG311" s="22"/>
@@ -33584,6 +33902,7 @@
     <row r="312" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B312" s="19"/>
       <c r="C312" s="19"/>
+      <c r="G312" s="40"/>
       <c r="BE312" s="22"/>
       <c r="BF312" s="22"/>
       <c r="BG312" s="22"/>
@@ -33688,6 +34007,7 @@
     <row r="313" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B313" s="19"/>
       <c r="C313" s="19"/>
+      <c r="G313" s="40"/>
       <c r="BE313" s="22"/>
       <c r="BF313" s="22"/>
       <c r="BG313" s="22"/>
@@ -33792,6 +34112,7 @@
     <row r="314" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B314" s="19"/>
       <c r="C314" s="19"/>
+      <c r="G314" s="40"/>
       <c r="BE314" s="22"/>
       <c r="BF314" s="22"/>
       <c r="BG314" s="22"/>
@@ -33896,6 +34217,7 @@
     <row r="315" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B315" s="19"/>
       <c r="C315" s="19"/>
+      <c r="G315" s="40"/>
       <c r="BE315" s="22"/>
       <c r="BF315" s="22"/>
       <c r="BG315" s="22"/>
@@ -34000,6 +34322,7 @@
     <row r="316" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B316" s="19"/>
       <c r="C316" s="19"/>
+      <c r="G316" s="40"/>
       <c r="BE316" s="22"/>
       <c r="BF316" s="22"/>
       <c r="BG316" s="22"/>
@@ -34104,6 +34427,7 @@
     <row r="317" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B317" s="19"/>
       <c r="C317" s="19"/>
+      <c r="G317" s="40"/>
       <c r="BE317" s="22"/>
       <c r="BF317" s="22"/>
       <c r="BG317" s="22"/>
@@ -34208,6 +34532,7 @@
     <row r="318" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B318" s="19"/>
       <c r="C318" s="19"/>
+      <c r="G318" s="40"/>
       <c r="BE318" s="22"/>
       <c r="BF318" s="22"/>
       <c r="BG318" s="22"/>
@@ -34312,6 +34637,7 @@
     <row r="319" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B319" s="19"/>
       <c r="C319" s="19"/>
+      <c r="G319" s="40"/>
       <c r="BE319" s="22"/>
       <c r="BF319" s="22"/>
       <c r="BG319" s="22"/>
@@ -34416,6 +34742,7 @@
     <row r="320" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B320" s="19"/>
       <c r="C320" s="19"/>
+      <c r="G320" s="40"/>
       <c r="BE320" s="22"/>
       <c r="BF320" s="22"/>
       <c r="BG320" s="22"/>
@@ -34520,6 +34847,7 @@
     <row r="321" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B321" s="19"/>
       <c r="C321" s="19"/>
+      <c r="G321" s="40"/>
       <c r="BE321" s="22"/>
       <c r="BF321" s="22"/>
       <c r="BG321" s="22"/>
@@ -34624,6 +34952,7 @@
     <row r="322" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B322" s="19"/>
       <c r="C322" s="19"/>
+      <c r="G322" s="40"/>
       <c r="BE322" s="22"/>
       <c r="BF322" s="22"/>
       <c r="BG322" s="22"/>
@@ -34728,6 +35057,7 @@
     <row r="323" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B323" s="19"/>
       <c r="C323" s="19"/>
+      <c r="G323" s="40"/>
       <c r="BE323" s="22"/>
       <c r="BF323" s="22"/>
       <c r="BG323" s="22"/>
@@ -34832,6 +35162,7 @@
     <row r="324" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B324" s="19"/>
       <c r="C324" s="19"/>
+      <c r="G324" s="40"/>
       <c r="BE324" s="22"/>
       <c r="BF324" s="22"/>
       <c r="BG324" s="22"/>
@@ -34936,6 +35267,7 @@
     <row r="325" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B325" s="19"/>
       <c r="C325" s="19"/>
+      <c r="G325" s="40"/>
       <c r="BE325" s="22"/>
       <c r="BF325" s="22"/>
       <c r="BG325" s="22"/>
@@ -35040,6 +35372,7 @@
     <row r="326" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B326" s="19"/>
       <c r="C326" s="19"/>
+      <c r="G326" s="40"/>
       <c r="BE326" s="22"/>
       <c r="BF326" s="22"/>
       <c r="BG326" s="22"/>
@@ -35144,6 +35477,7 @@
     <row r="327" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B327" s="19"/>
       <c r="C327" s="19"/>
+      <c r="G327" s="40"/>
       <c r="BE327" s="22"/>
       <c r="BF327" s="22"/>
       <c r="BG327" s="22"/>
@@ -35248,6 +35582,7 @@
     <row r="328" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B328" s="19"/>
       <c r="C328" s="19"/>
+      <c r="G328" s="40"/>
       <c r="BE328" s="22"/>
       <c r="BF328" s="22"/>
       <c r="BG328" s="22"/>
@@ -35352,6 +35687,7 @@
     <row r="329" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B329" s="19"/>
       <c r="C329" s="19"/>
+      <c r="G329" s="40"/>
       <c r="BE329" s="22"/>
       <c r="BF329" s="22"/>
       <c r="BG329" s="22"/>
@@ -35456,6 +35792,7 @@
     <row r="330" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B330" s="19"/>
       <c r="C330" s="19"/>
+      <c r="G330" s="40"/>
       <c r="BE330" s="22"/>
       <c r="BF330" s="22"/>
       <c r="BG330" s="22"/>
@@ -35560,6 +35897,7 @@
     <row r="331" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B331" s="19"/>
       <c r="C331" s="19"/>
+      <c r="G331" s="40"/>
       <c r="BE331" s="22"/>
       <c r="BF331" s="22"/>
       <c r="BG331" s="22"/>
@@ -35664,6 +36002,7 @@
     <row r="332" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B332" s="19"/>
       <c r="C332" s="19"/>
+      <c r="G332" s="40"/>
       <c r="BE332" s="22"/>
       <c r="BF332" s="22"/>
       <c r="BG332" s="22"/>
@@ -35768,6 +36107,7 @@
     <row r="333" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B333" s="19"/>
       <c r="C333" s="19"/>
+      <c r="G333" s="40"/>
       <c r="BE333" s="22"/>
       <c r="BF333" s="22"/>
       <c r="BG333" s="22"/>
@@ -35872,6 +36212,7 @@
     <row r="334" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B334" s="19"/>
       <c r="C334" s="19"/>
+      <c r="G334" s="40"/>
       <c r="BE334" s="22"/>
       <c r="BF334" s="22"/>
       <c r="BG334" s="22"/>
@@ -35976,6 +36317,7 @@
     <row r="335" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B335" s="19"/>
       <c r="C335" s="19"/>
+      <c r="G335" s="40"/>
       <c r="BE335" s="22"/>
       <c r="BF335" s="22"/>
       <c r="BG335" s="22"/>
@@ -36080,6 +36422,7 @@
     <row r="336" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B336" s="19"/>
       <c r="C336" s="19"/>
+      <c r="G336" s="40"/>
       <c r="BE336" s="22"/>
       <c r="BF336" s="22"/>
       <c r="BG336" s="22"/>
@@ -36184,6 +36527,7 @@
     <row r="337" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B337" s="19"/>
       <c r="C337" s="19"/>
+      <c r="G337" s="40"/>
       <c r="BE337" s="22"/>
       <c r="BF337" s="22"/>
       <c r="BG337" s="22"/>
@@ -36288,6 +36632,7 @@
     <row r="338" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B338" s="19"/>
       <c r="C338" s="19"/>
+      <c r="G338" s="40"/>
       <c r="BE338" s="22"/>
       <c r="BF338" s="22"/>
       <c r="BG338" s="22"/>
@@ -36392,6 +36737,7 @@
     <row r="339" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B339" s="19"/>
       <c r="C339" s="19"/>
+      <c r="G339" s="40"/>
       <c r="BE339" s="22"/>
       <c r="BF339" s="22"/>
       <c r="BG339" s="22"/>
@@ -36496,6 +36842,7 @@
     <row r="340" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B340" s="19"/>
       <c r="C340" s="19"/>
+      <c r="G340" s="40"/>
       <c r="BE340" s="22"/>
       <c r="BF340" s="22"/>
       <c r="BG340" s="22"/>
@@ -36600,6 +36947,7 @@
     <row r="341" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B341" s="19"/>
       <c r="C341" s="19"/>
+      <c r="G341" s="40"/>
       <c r="BE341" s="22"/>
       <c r="BF341" s="22"/>
       <c r="BG341" s="22"/>
@@ -36704,6 +37052,7 @@
     <row r="342" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B342" s="19"/>
       <c r="C342" s="19"/>
+      <c r="G342" s="40"/>
       <c r="BE342" s="22"/>
       <c r="BF342" s="22"/>
       <c r="BG342" s="22"/>
@@ -36808,6 +37157,7 @@
     <row r="343" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B343" s="19"/>
       <c r="C343" s="19"/>
+      <c r="G343" s="40"/>
       <c r="BE343" s="22"/>
       <c r="BF343" s="22"/>
       <c r="BG343" s="22"/>
@@ -36912,6 +37262,7 @@
     <row r="344" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B344" s="19"/>
       <c r="C344" s="19"/>
+      <c r="G344" s="40"/>
       <c r="BE344" s="22"/>
       <c r="BF344" s="22"/>
       <c r="BG344" s="22"/>
@@ -37016,6 +37367,7 @@
     <row r="345" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B345" s="19"/>
       <c r="C345" s="19"/>
+      <c r="G345" s="40"/>
       <c r="BE345" s="22"/>
       <c r="BF345" s="22"/>
       <c r="BG345" s="22"/>
@@ -37120,6 +37472,7 @@
     <row r="346" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B346" s="19"/>
       <c r="C346" s="19"/>
+      <c r="G346" s="40"/>
       <c r="BE346" s="22"/>
       <c r="BF346" s="22"/>
       <c r="BG346" s="22"/>
@@ -37224,6 +37577,7 @@
     <row r="347" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B347" s="19"/>
       <c r="C347" s="19"/>
+      <c r="G347" s="40"/>
       <c r="BE347" s="22"/>
       <c r="BF347" s="22"/>
       <c r="BG347" s="22"/>
@@ -37328,6 +37682,7 @@
     <row r="348" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B348" s="19"/>
       <c r="C348" s="19"/>
+      <c r="G348" s="40"/>
       <c r="BE348" s="22"/>
       <c r="BF348" s="22"/>
       <c r="BG348" s="22"/>
@@ -37432,6 +37787,7 @@
     <row r="349" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B349" s="19"/>
       <c r="C349" s="19"/>
+      <c r="G349" s="40"/>
       <c r="BE349" s="22"/>
       <c r="BF349" s="22"/>
       <c r="BG349" s="22"/>
@@ -37536,6 +37892,7 @@
     <row r="350" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B350" s="19"/>
       <c r="C350" s="19"/>
+      <c r="G350" s="40"/>
       <c r="BE350" s="22"/>
       <c r="BF350" s="22"/>
       <c r="BG350" s="22"/>
@@ -37640,6 +37997,7 @@
     <row r="351" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B351" s="19"/>
       <c r="C351" s="19"/>
+      <c r="G351" s="40"/>
       <c r="BE351" s="22"/>
       <c r="BF351" s="22"/>
       <c r="BG351" s="22"/>
@@ -37744,6 +38102,7 @@
     <row r="352" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B352" s="19"/>
       <c r="C352" s="19"/>
+      <c r="G352" s="40"/>
       <c r="BE352" s="22"/>
       <c r="BF352" s="22"/>
       <c r="BG352" s="22"/>
@@ -37848,6 +38207,7 @@
     <row r="353" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B353" s="19"/>
       <c r="C353" s="19"/>
+      <c r="G353" s="40"/>
       <c r="BE353" s="22"/>
       <c r="BF353" s="22"/>
       <c r="BG353" s="22"/>
@@ -37952,6 +38312,7 @@
     <row r="354" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B354" s="19"/>
       <c r="C354" s="19"/>
+      <c r="G354" s="40"/>
       <c r="BE354" s="22"/>
       <c r="BF354" s="22"/>
       <c r="BG354" s="22"/>
@@ -38056,6 +38417,7 @@
     <row r="355" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B355" s="19"/>
       <c r="C355" s="19"/>
+      <c r="G355" s="40"/>
       <c r="BE355" s="22"/>
       <c r="BF355" s="22"/>
       <c r="BG355" s="22"/>
@@ -38160,6 +38522,7 @@
     <row r="356" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B356" s="19"/>
       <c r="C356" s="19"/>
+      <c r="G356" s="40"/>
       <c r="BE356" s="22"/>
       <c r="BF356" s="22"/>
       <c r="BG356" s="22"/>
@@ -38264,6 +38627,7 @@
     <row r="357" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B357" s="19"/>
       <c r="C357" s="19"/>
+      <c r="G357" s="40"/>
       <c r="BE357" s="22"/>
       <c r="BF357" s="22"/>
       <c r="BG357" s="22"/>
@@ -38368,6 +38732,7 @@
     <row r="358" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B358" s="19"/>
       <c r="C358" s="19"/>
+      <c r="G358" s="40"/>
       <c r="BE358" s="22"/>
       <c r="BF358" s="22"/>
       <c r="BG358" s="22"/>
@@ -38472,6 +38837,7 @@
     <row r="359" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B359" s="19"/>
       <c r="C359" s="19"/>
+      <c r="G359" s="40"/>
       <c r="BE359" s="22"/>
       <c r="BF359" s="22"/>
       <c r="BG359" s="22"/>
@@ -38576,6 +38942,7 @@
     <row r="360" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B360" s="19"/>
       <c r="C360" s="19"/>
+      <c r="G360" s="40"/>
       <c r="BE360" s="22"/>
       <c r="BF360" s="22"/>
       <c r="BG360" s="22"/>
@@ -38680,6 +39047,7 @@
     <row r="361" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B361" s="19"/>
       <c r="C361" s="19"/>
+      <c r="G361" s="40"/>
       <c r="BE361" s="22"/>
       <c r="BF361" s="22"/>
       <c r="BG361" s="22"/>
@@ -38784,6 +39152,7 @@
     <row r="362" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B362" s="19"/>
       <c r="C362" s="19"/>
+      <c r="G362" s="40"/>
       <c r="BE362" s="22"/>
       <c r="BF362" s="22"/>
       <c r="BG362" s="22"/>
@@ -38888,6 +39257,7 @@
     <row r="363" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B363" s="19"/>
       <c r="C363" s="19"/>
+      <c r="G363" s="40"/>
       <c r="BE363" s="22"/>
       <c r="BF363" s="22"/>
       <c r="BG363" s="22"/>
@@ -38992,6 +39362,7 @@
     <row r="364" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B364" s="19"/>
       <c r="C364" s="19"/>
+      <c r="G364" s="40"/>
       <c r="BE364" s="22"/>
       <c r="BF364" s="22"/>
       <c r="BG364" s="22"/>
@@ -39096,6 +39467,7 @@
     <row r="365" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B365" s="19"/>
       <c r="C365" s="19"/>
+      <c r="G365" s="40"/>
       <c r="BE365" s="22"/>
       <c r="BF365" s="22"/>
       <c r="BG365" s="22"/>
@@ -39200,6 +39572,7 @@
     <row r="366" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B366" s="19"/>
       <c r="C366" s="19"/>
+      <c r="G366" s="40"/>
       <c r="BE366" s="22"/>
       <c r="BF366" s="22"/>
       <c r="BG366" s="22"/>
@@ -39304,6 +39677,7 @@
     <row r="367" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B367" s="19"/>
       <c r="C367" s="19"/>
+      <c r="G367" s="40"/>
       <c r="BE367" s="22"/>
       <c r="BF367" s="22"/>
       <c r="BG367" s="22"/>
@@ -39408,6 +39782,7 @@
     <row r="368" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B368" s="19"/>
       <c r="C368" s="19"/>
+      <c r="G368" s="40"/>
       <c r="BE368" s="22"/>
       <c r="BF368" s="22"/>
       <c r="BG368" s="22"/>
@@ -39512,6 +39887,7 @@
     <row r="369" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B369" s="19"/>
       <c r="C369" s="19"/>
+      <c r="G369" s="40"/>
       <c r="BE369" s="22"/>
       <c r="BF369" s="22"/>
       <c r="BG369" s="22"/>
@@ -39616,6 +39992,7 @@
     <row r="370" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B370" s="19"/>
       <c r="C370" s="19"/>
+      <c r="G370" s="40"/>
       <c r="BE370" s="22"/>
       <c r="BF370" s="22"/>
       <c r="BG370" s="22"/>
@@ -39720,6 +40097,7 @@
     <row r="371" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B371" s="19"/>
       <c r="C371" s="19"/>
+      <c r="G371" s="40"/>
       <c r="BE371" s="22"/>
       <c r="BF371" s="22"/>
       <c r="BG371" s="22"/>
@@ -39824,6 +40202,7 @@
     <row r="372" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B372" s="19"/>
       <c r="C372" s="19"/>
+      <c r="G372" s="40"/>
       <c r="BE372" s="22"/>
       <c r="BF372" s="22"/>
       <c r="BG372" s="22"/>
@@ -39928,6 +40307,7 @@
     <row r="373" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B373" s="19"/>
       <c r="C373" s="19"/>
+      <c r="G373" s="40"/>
       <c r="BE373" s="22"/>
       <c r="BF373" s="22"/>
       <c r="BG373" s="22"/>
@@ -40032,6 +40412,7 @@
     <row r="374" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B374" s="19"/>
       <c r="C374" s="19"/>
+      <c r="G374" s="40"/>
       <c r="BE374" s="22"/>
       <c r="BF374" s="22"/>
       <c r="BG374" s="22"/>
@@ -40136,6 +40517,7 @@
     <row r="375" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B375" s="19"/>
       <c r="C375" s="19"/>
+      <c r="G375" s="40"/>
       <c r="BE375" s="22"/>
       <c r="BF375" s="22"/>
       <c r="BG375" s="22"/>
@@ -40240,6 +40622,7 @@
     <row r="376" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B376" s="19"/>
       <c r="C376" s="19"/>
+      <c r="G376" s="40"/>
       <c r="BE376" s="22"/>
       <c r="BF376" s="22"/>
       <c r="BG376" s="22"/>
@@ -40344,6 +40727,7 @@
     <row r="377" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B377" s="19"/>
       <c r="C377" s="19"/>
+      <c r="G377" s="40"/>
       <c r="BE377" s="22"/>
       <c r="BF377" s="22"/>
       <c r="BG377" s="22"/>
@@ -40448,6 +40832,7 @@
     <row r="378" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B378" s="19"/>
       <c r="C378" s="19"/>
+      <c r="G378" s="40"/>
       <c r="BE378" s="22"/>
       <c r="BF378" s="22"/>
       <c r="BG378" s="22"/>
@@ -40552,6 +40937,7 @@
     <row r="379" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B379" s="19"/>
       <c r="C379" s="19"/>
+      <c r="G379" s="40"/>
       <c r="BE379" s="22"/>
       <c r="BF379" s="22"/>
       <c r="BG379" s="22"/>
@@ -40656,6 +41042,7 @@
     <row r="380" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B380" s="19"/>
       <c r="C380" s="19"/>
+      <c r="G380" s="40"/>
       <c r="BE380" s="22"/>
       <c r="BF380" s="22"/>
       <c r="BG380" s="22"/>
@@ -40760,6 +41147,7 @@
     <row r="381" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B381" s="19"/>
       <c r="C381" s="19"/>
+      <c r="G381" s="40"/>
       <c r="BE381" s="22"/>
       <c r="BF381" s="22"/>
       <c r="BG381" s="22"/>
@@ -40864,6 +41252,7 @@
     <row r="382" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B382" s="19"/>
       <c r="C382" s="19"/>
+      <c r="G382" s="40"/>
       <c r="BE382" s="22"/>
       <c r="BF382" s="22"/>
       <c r="BG382" s="22"/>
@@ -40968,6 +41357,7 @@
     <row r="383" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B383" s="19"/>
       <c r="C383" s="19"/>
+      <c r="G383" s="40"/>
       <c r="BE383" s="22"/>
       <c r="BF383" s="22"/>
       <c r="BG383" s="22"/>
@@ -41072,6 +41462,7 @@
     <row r="384" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B384" s="19"/>
       <c r="C384" s="19"/>
+      <c r="G384" s="40"/>
       <c r="BE384" s="22"/>
       <c r="BF384" s="22"/>
       <c r="BG384" s="22"/>
@@ -41176,6 +41567,7 @@
     <row r="385" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B385" s="19"/>
       <c r="C385" s="19"/>
+      <c r="G385" s="40"/>
       <c r="BE385" s="22"/>
       <c r="BF385" s="22"/>
       <c r="BG385" s="22"/>
@@ -41280,6 +41672,7 @@
     <row r="386" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B386" s="19"/>
       <c r="C386" s="19"/>
+      <c r="G386" s="40"/>
       <c r="BE386" s="22"/>
       <c r="BF386" s="22"/>
       <c r="BG386" s="22"/>
@@ -41384,6 +41777,7 @@
     <row r="387" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B387" s="19"/>
       <c r="C387" s="19"/>
+      <c r="G387" s="40"/>
       <c r="BE387" s="22"/>
       <c r="BF387" s="22"/>
       <c r="BG387" s="22"/>
@@ -41488,6 +41882,7 @@
     <row r="388" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B388" s="19"/>
       <c r="C388" s="19"/>
+      <c r="G388" s="40"/>
       <c r="BE388" s="22"/>
       <c r="BF388" s="22"/>
       <c r="BG388" s="22"/>
@@ -41592,6 +41987,7 @@
     <row r="389" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B389" s="19"/>
       <c r="C389" s="19"/>
+      <c r="G389" s="40"/>
       <c r="BE389" s="22"/>
       <c r="BF389" s="22"/>
       <c r="BG389" s="22"/>
@@ -41696,6 +42092,7 @@
     <row r="390" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B390" s="19"/>
       <c r="C390" s="19"/>
+      <c r="G390" s="40"/>
       <c r="BE390" s="22"/>
       <c r="BF390" s="22"/>
       <c r="BG390" s="22"/>
@@ -41800,6 +42197,7 @@
     <row r="391" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B391" s="19"/>
       <c r="C391" s="19"/>
+      <c r="G391" s="40"/>
       <c r="BE391" s="22"/>
       <c r="BF391" s="22"/>
       <c r="BG391" s="22"/>
@@ -41904,6 +42302,7 @@
     <row r="392" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B392" s="19"/>
       <c r="C392" s="19"/>
+      <c r="G392" s="40"/>
       <c r="BE392" s="22"/>
       <c r="BF392" s="22"/>
       <c r="BG392" s="22"/>
@@ -42008,6 +42407,7 @@
     <row r="393" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B393" s="19"/>
       <c r="C393" s="19"/>
+      <c r="G393" s="40"/>
       <c r="BE393" s="22"/>
       <c r="BF393" s="22"/>
       <c r="BG393" s="22"/>
@@ -42112,6 +42512,7 @@
     <row r="394" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B394" s="19"/>
       <c r="C394" s="19"/>
+      <c r="G394" s="40"/>
       <c r="BE394" s="22"/>
       <c r="BF394" s="22"/>
       <c r="BG394" s="22"/>
@@ -42216,6 +42617,7 @@
     <row r="395" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B395" s="19"/>
       <c r="C395" s="19"/>
+      <c r="G395" s="40"/>
       <c r="BE395" s="22"/>
       <c r="BF395" s="22"/>
       <c r="BG395" s="22"/>
@@ -42320,6 +42722,7 @@
     <row r="396" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B396" s="19"/>
       <c r="C396" s="19"/>
+      <c r="G396" s="40"/>
       <c r="BE396" s="22"/>
       <c r="BF396" s="22"/>
       <c r="BG396" s="22"/>
@@ -42424,6 +42827,7 @@
     <row r="397" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B397" s="19"/>
       <c r="C397" s="19"/>
+      <c r="G397" s="40"/>
       <c r="BE397" s="22"/>
       <c r="BF397" s="22"/>
       <c r="BG397" s="22"/>
@@ -42528,6 +42932,7 @@
     <row r="398" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B398" s="19"/>
       <c r="C398" s="19"/>
+      <c r="G398" s="40"/>
       <c r="BE398" s="22"/>
       <c r="BF398" s="22"/>
       <c r="BG398" s="22"/>
@@ -42632,6 +43037,7 @@
     <row r="399" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B399" s="19"/>
       <c r="C399" s="19"/>
+      <c r="G399" s="40"/>
       <c r="BE399" s="22"/>
       <c r="BF399" s="22"/>
       <c r="BG399" s="22"/>
@@ -42736,6 +43142,7 @@
     <row r="400" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B400" s="19"/>
       <c r="C400" s="19"/>
+      <c r="G400" s="40"/>
       <c r="BE400" s="22"/>
       <c r="BF400" s="22"/>
       <c r="BG400" s="22"/>
@@ -42840,6 +43247,7 @@
     <row r="401" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B401" s="19"/>
       <c r="C401" s="19"/>
+      <c r="G401" s="40"/>
       <c r="BE401" s="22"/>
       <c r="BF401" s="22"/>
       <c r="BG401" s="22"/>
@@ -42944,6 +43352,7 @@
     <row r="402" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B402" s="19"/>
       <c r="C402" s="19"/>
+      <c r="G402" s="40"/>
       <c r="BE402" s="22"/>
       <c r="BF402" s="22"/>
       <c r="BG402" s="22"/>
@@ -43048,6 +43457,7 @@
     <row r="403" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B403" s="19"/>
       <c r="C403" s="19"/>
+      <c r="G403" s="40"/>
       <c r="BE403" s="22"/>
       <c r="BF403" s="22"/>
       <c r="BG403" s="22"/>
@@ -43152,6 +43562,7 @@
     <row r="404" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B404" s="19"/>
       <c r="C404" s="19"/>
+      <c r="G404" s="40"/>
       <c r="BE404" s="22"/>
       <c r="BF404" s="22"/>
       <c r="BG404" s="22"/>
@@ -43256,6 +43667,7 @@
     <row r="405" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B405" s="19"/>
       <c r="C405" s="19"/>
+      <c r="G405" s="40"/>
       <c r="BE405" s="22"/>
       <c r="BF405" s="22"/>
       <c r="BG405" s="22"/>
@@ -43360,6 +43772,7 @@
     <row r="406" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B406" s="19"/>
       <c r="C406" s="19"/>
+      <c r="G406" s="40"/>
       <c r="BE406" s="22"/>
       <c r="BF406" s="22"/>
       <c r="BG406" s="22"/>
@@ -43464,6 +43877,7 @@
     <row r="407" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B407" s="19"/>
       <c r="C407" s="19"/>
+      <c r="G407" s="40"/>
       <c r="BE407" s="22"/>
       <c r="BF407" s="22"/>
       <c r="BG407" s="22"/>
@@ -43568,6 +43982,7 @@
     <row r="408" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B408" s="19"/>
       <c r="C408" s="19"/>
+      <c r="G408" s="40"/>
       <c r="BE408" s="22"/>
       <c r="BF408" s="22"/>
       <c r="BG408" s="22"/>
@@ -43672,6 +44087,7 @@
     <row r="409" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B409" s="19"/>
       <c r="C409" s="19"/>
+      <c r="G409" s="40"/>
       <c r="BE409" s="22"/>
       <c r="BF409" s="22"/>
       <c r="BG409" s="22"/>
@@ -43776,6 +44192,7 @@
     <row r="410" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B410" s="19"/>
       <c r="C410" s="19"/>
+      <c r="G410" s="40"/>
       <c r="BE410" s="22"/>
       <c r="BF410" s="22"/>
       <c r="BG410" s="22"/>
@@ -43880,6 +44297,7 @@
     <row r="411" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B411" s="19"/>
       <c r="C411" s="19"/>
+      <c r="G411" s="40"/>
       <c r="BE411" s="22"/>
       <c r="BF411" s="22"/>
       <c r="BG411" s="22"/>
@@ -43984,6 +44402,7 @@
     <row r="412" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B412" s="19"/>
       <c r="C412" s="19"/>
+      <c r="G412" s="40"/>
       <c r="BE412" s="22"/>
       <c r="BF412" s="22"/>
       <c r="BG412" s="22"/>
@@ -44088,6 +44507,7 @@
     <row r="413" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B413" s="19"/>
       <c r="C413" s="19"/>
+      <c r="G413" s="40"/>
       <c r="BE413" s="22"/>
       <c r="BF413" s="22"/>
       <c r="BG413" s="22"/>
@@ -44192,6 +44612,7 @@
     <row r="414" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B414" s="19"/>
       <c r="C414" s="19"/>
+      <c r="G414" s="40"/>
       <c r="BE414" s="22"/>
       <c r="BF414" s="22"/>
       <c r="BG414" s="22"/>
@@ -44296,6 +44717,7 @@
     <row r="415" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B415" s="19"/>
       <c r="C415" s="19"/>
+      <c r="G415" s="40"/>
       <c r="BE415" s="22"/>
       <c r="BF415" s="22"/>
       <c r="BG415" s="22"/>
@@ -44400,6 +44822,7 @@
     <row r="416" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B416" s="19"/>
       <c r="C416" s="19"/>
+      <c r="G416" s="40"/>
       <c r="BE416" s="22"/>
       <c r="BF416" s="22"/>
       <c r="BG416" s="22"/>
@@ -44504,6 +44927,7 @@
     <row r="417" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B417" s="19"/>
       <c r="C417" s="19"/>
+      <c r="G417" s="40"/>
       <c r="BE417" s="22"/>
       <c r="BF417" s="22"/>
       <c r="BG417" s="22"/>
@@ -44608,6 +45032,7 @@
     <row r="418" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B418" s="19"/>
       <c r="C418" s="19"/>
+      <c r="G418" s="40"/>
       <c r="BE418" s="22"/>
       <c r="BF418" s="22"/>
       <c r="BG418" s="22"/>
@@ -44712,6 +45137,7 @@
     <row r="419" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B419" s="19"/>
       <c r="C419" s="19"/>
+      <c r="G419" s="40"/>
       <c r="BE419" s="22"/>
       <c r="BF419" s="22"/>
       <c r="BG419" s="22"/>
@@ -44816,6 +45242,7 @@
     <row r="420" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B420" s="19"/>
       <c r="C420" s="19"/>
+      <c r="G420" s="40"/>
       <c r="BE420" s="22"/>
       <c r="BF420" s="22"/>
       <c r="BG420" s="22"/>
@@ -44920,6 +45347,7 @@
     <row r="421" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B421" s="19"/>
       <c r="C421" s="19"/>
+      <c r="G421" s="40"/>
       <c r="BE421" s="22"/>
       <c r="BF421" s="22"/>
       <c r="BG421" s="22"/>
@@ -45024,6 +45452,7 @@
     <row r="422" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B422" s="19"/>
       <c r="C422" s="19"/>
+      <c r="G422" s="40"/>
       <c r="BE422" s="22"/>
       <c r="BF422" s="22"/>
       <c r="BG422" s="22"/>
@@ -45128,6 +45557,7 @@
     <row r="423" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B423" s="19"/>
       <c r="C423" s="19"/>
+      <c r="G423" s="40"/>
       <c r="BE423" s="22"/>
       <c r="BF423" s="22"/>
       <c r="BG423" s="22"/>
@@ -45232,6 +45662,7 @@
     <row r="424" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B424" s="19"/>
       <c r="C424" s="19"/>
+      <c r="G424" s="40"/>
       <c r="BE424" s="22"/>
       <c r="BF424" s="22"/>
       <c r="BG424" s="22"/>
@@ -45336,6 +45767,7 @@
     <row r="425" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B425" s="19"/>
       <c r="C425" s="19"/>
+      <c r="G425" s="40"/>
       <c r="BE425" s="22"/>
       <c r="BF425" s="22"/>
       <c r="BG425" s="22"/>
@@ -45440,6 +45872,7 @@
     <row r="426" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B426" s="19"/>
       <c r="C426" s="19"/>
+      <c r="G426" s="40"/>
       <c r="BE426" s="22"/>
       <c r="BF426" s="22"/>
       <c r="BG426" s="22"/>
@@ -45544,6 +45977,7 @@
     <row r="427" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B427" s="19"/>
       <c r="C427" s="19"/>
+      <c r="G427" s="40"/>
       <c r="BE427" s="22"/>
       <c r="BF427" s="22"/>
       <c r="BG427" s="22"/>
@@ -45648,6 +46082,7 @@
     <row r="428" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B428" s="19"/>
       <c r="C428" s="19"/>
+      <c r="G428" s="40"/>
       <c r="BE428" s="22"/>
       <c r="BF428" s="22"/>
       <c r="BG428" s="22"/>
@@ -45752,6 +46187,7 @@
     <row r="429" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B429" s="19"/>
       <c r="C429" s="19"/>
+      <c r="G429" s="40"/>
       <c r="BE429" s="22"/>
       <c r="BF429" s="22"/>
       <c r="BG429" s="22"/>
@@ -45856,6 +46292,7 @@
     <row r="430" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B430" s="19"/>
       <c r="C430" s="19"/>
+      <c r="G430" s="40"/>
       <c r="BE430" s="22"/>
       <c r="BF430" s="22"/>
       <c r="BG430" s="22"/>
@@ -45960,6 +46397,7 @@
     <row r="431" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B431" s="19"/>
       <c r="C431" s="19"/>
+      <c r="G431" s="40"/>
       <c r="BE431" s="22"/>
       <c r="BF431" s="22"/>
       <c r="BG431" s="22"/>
@@ -46064,6 +46502,7 @@
     <row r="432" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B432" s="19"/>
       <c r="C432" s="19"/>
+      <c r="G432" s="40"/>
       <c r="BE432" s="22"/>
       <c r="BF432" s="22"/>
       <c r="BG432" s="22"/>
@@ -46168,6 +46607,7 @@
     <row r="433" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B433" s="19"/>
       <c r="C433" s="19"/>
+      <c r="G433" s="40"/>
       <c r="BE433" s="22"/>
       <c r="BF433" s="22"/>
       <c r="BG433" s="22"/>
@@ -46272,6 +46712,7 @@
     <row r="434" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B434" s="19"/>
       <c r="C434" s="19"/>
+      <c r="G434" s="40"/>
       <c r="BE434" s="22"/>
       <c r="BF434" s="22"/>
       <c r="BG434" s="22"/>
@@ -46376,6 +46817,7 @@
     <row r="435" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B435" s="19"/>
       <c r="C435" s="19"/>
+      <c r="G435" s="40"/>
       <c r="BE435" s="22"/>
       <c r="BF435" s="22"/>
       <c r="BG435" s="22"/>
@@ -46480,6 +46922,7 @@
     <row r="436" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B436" s="19"/>
       <c r="C436" s="19"/>
+      <c r="G436" s="40"/>
       <c r="BE436" s="22"/>
       <c r="BF436" s="22"/>
       <c r="BG436" s="22"/>
@@ -46584,6 +47027,7 @@
     <row r="437" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B437" s="19"/>
       <c r="C437" s="19"/>
+      <c r="G437" s="40"/>
       <c r="BE437" s="22"/>
       <c r="BF437" s="22"/>
       <c r="BG437" s="22"/>
@@ -46688,6 +47132,7 @@
     <row r="438" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B438" s="19"/>
       <c r="C438" s="19"/>
+      <c r="G438" s="40"/>
       <c r="BE438" s="22"/>
       <c r="BF438" s="22"/>
       <c r="BG438" s="22"/>
@@ -46792,6 +47237,7 @@
     <row r="439" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B439" s="19"/>
       <c r="C439" s="19"/>
+      <c r="G439" s="40"/>
       <c r="BE439" s="22"/>
       <c r="BF439" s="22"/>
       <c r="BG439" s="22"/>
@@ -46896,6 +47342,7 @@
     <row r="440" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B440" s="19"/>
       <c r="C440" s="19"/>
+      <c r="G440" s="40"/>
       <c r="BE440" s="22"/>
       <c r="BF440" s="22"/>
       <c r="BG440" s="22"/>
@@ -47000,6 +47447,7 @@
     <row r="441" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B441" s="19"/>
       <c r="C441" s="19"/>
+      <c r="G441" s="40"/>
       <c r="BE441" s="22"/>
       <c r="BF441" s="22"/>
       <c r="BG441" s="22"/>
@@ -47104,6 +47552,7 @@
     <row r="442" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B442" s="19"/>
       <c r="C442" s="19"/>
+      <c r="G442" s="40"/>
       <c r="BE442" s="22"/>
       <c r="BF442" s="22"/>
       <c r="BG442" s="22"/>
@@ -47208,6 +47657,7 @@
     <row r="443" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B443" s="19"/>
       <c r="C443" s="19"/>
+      <c r="G443" s="40"/>
       <c r="BE443" s="22"/>
       <c r="BF443" s="22"/>
       <c r="BG443" s="22"/>
@@ -47312,6 +47762,7 @@
     <row r="444" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B444" s="19"/>
       <c r="C444" s="19"/>
+      <c r="G444" s="40"/>
       <c r="BE444" s="22"/>
       <c r="BF444" s="22"/>
       <c r="BG444" s="22"/>
@@ -47416,6 +47867,7 @@
     <row r="445" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B445" s="19"/>
       <c r="C445" s="19"/>
+      <c r="G445" s="40"/>
       <c r="BE445" s="22"/>
       <c r="BF445" s="22"/>
       <c r="BG445" s="22"/>
@@ -47520,6 +47972,7 @@
     <row r="446" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B446" s="19"/>
       <c r="C446" s="19"/>
+      <c r="G446" s="40"/>
       <c r="BE446" s="22"/>
       <c r="BF446" s="22"/>
       <c r="BG446" s="22"/>
@@ -47624,6 +48077,7 @@
     <row r="447" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B447" s="19"/>
       <c r="C447" s="19"/>
+      <c r="G447" s="40"/>
       <c r="BE447" s="22"/>
       <c r="BF447" s="22"/>
       <c r="BG447" s="22"/>
@@ -47728,6 +48182,7 @@
     <row r="448" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B448" s="19"/>
       <c r="C448" s="19"/>
+      <c r="G448" s="40"/>
       <c r="BE448" s="22"/>
       <c r="BF448" s="22"/>
       <c r="BG448" s="22"/>
@@ -47832,6 +48287,7 @@
     <row r="449" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B449" s="19"/>
       <c r="C449" s="19"/>
+      <c r="G449" s="40"/>
       <c r="BE449" s="22"/>
       <c r="BF449" s="22"/>
       <c r="BG449" s="22"/>
@@ -47936,6 +48392,7 @@
     <row r="450" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B450" s="19"/>
       <c r="C450" s="19"/>
+      <c r="G450" s="40"/>
       <c r="BE450" s="22"/>
       <c r="BF450" s="22"/>
       <c r="BG450" s="22"/>
@@ -48040,6 +48497,7 @@
     <row r="451" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B451" s="19"/>
       <c r="C451" s="19"/>
+      <c r="G451" s="40"/>
       <c r="BE451" s="22"/>
       <c r="BF451" s="22"/>
       <c r="BG451" s="22"/>
@@ -48144,6 +48602,7 @@
     <row r="452" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B452" s="19"/>
       <c r="C452" s="19"/>
+      <c r="G452" s="40"/>
       <c r="BE452" s="22"/>
       <c r="BF452" s="22"/>
       <c r="BG452" s="22"/>
@@ -48248,6 +48707,7 @@
     <row r="453" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B453" s="19"/>
       <c r="C453" s="19"/>
+      <c r="G453" s="40"/>
       <c r="BE453" s="22"/>
       <c r="BF453" s="22"/>
       <c r="BG453" s="22"/>
@@ -48352,6 +48812,7 @@
     <row r="454" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B454" s="19"/>
       <c r="C454" s="19"/>
+      <c r="G454" s="40"/>
       <c r="BE454" s="22"/>
       <c r="BF454" s="22"/>
       <c r="BG454" s="22"/>
@@ -48456,6 +48917,7 @@
     <row r="455" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B455" s="19"/>
       <c r="C455" s="19"/>
+      <c r="G455" s="40"/>
       <c r="BE455" s="22"/>
       <c r="BF455" s="22"/>
       <c r="BG455" s="22"/>
@@ -48560,6 +49022,7 @@
     <row r="456" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B456" s="19"/>
       <c r="C456" s="19"/>
+      <c r="G456" s="40"/>
       <c r="BE456" s="22"/>
       <c r="BF456" s="22"/>
       <c r="BG456" s="22"/>
@@ -48664,6 +49127,7 @@
     <row r="457" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B457" s="19"/>
       <c r="C457" s="19"/>
+      <c r="G457" s="40"/>
       <c r="BE457" s="22"/>
       <c r="BF457" s="22"/>
       <c r="BG457" s="22"/>
@@ -48768,6 +49232,7 @@
     <row r="458" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B458" s="19"/>
       <c r="C458" s="19"/>
+      <c r="G458" s="40"/>
       <c r="BE458" s="22"/>
       <c r="BF458" s="22"/>
       <c r="BG458" s="22"/>
@@ -48872,6 +49337,7 @@
     <row r="459" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B459" s="19"/>
       <c r="C459" s="19"/>
+      <c r="G459" s="40"/>
       <c r="BE459" s="22"/>
       <c r="BF459" s="22"/>
       <c r="BG459" s="22"/>
@@ -48976,6 +49442,7 @@
     <row r="460" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B460" s="19"/>
       <c r="C460" s="19"/>
+      <c r="G460" s="40"/>
       <c r="BE460" s="22"/>
       <c r="BF460" s="22"/>
       <c r="BG460" s="22"/>
@@ -49080,6 +49547,7 @@
     <row r="461" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B461" s="19"/>
       <c r="C461" s="19"/>
+      <c r="G461" s="40"/>
       <c r="BE461" s="22"/>
       <c r="BF461" s="22"/>
       <c r="BG461" s="22"/>
@@ -49184,6 +49652,7 @@
     <row r="462" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B462" s="19"/>
       <c r="C462" s="19"/>
+      <c r="G462" s="40"/>
       <c r="BE462" s="22"/>
       <c r="BF462" s="22"/>
       <c r="BG462" s="22"/>
@@ -49288,6 +49757,7 @@
     <row r="463" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B463" s="19"/>
       <c r="C463" s="19"/>
+      <c r="G463" s="40"/>
       <c r="BE463" s="22"/>
       <c r="BF463" s="22"/>
       <c r="BG463" s="22"/>
@@ -49392,6 +49862,7 @@
     <row r="464" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B464" s="19"/>
       <c r="C464" s="19"/>
+      <c r="G464" s="40"/>
       <c r="BE464" s="22"/>
       <c r="BF464" s="22"/>
       <c r="BG464" s="22"/>
@@ -49496,6 +49967,7 @@
     <row r="465" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B465" s="19"/>
       <c r="C465" s="19"/>
+      <c r="G465" s="40"/>
       <c r="BE465" s="22"/>
       <c r="BF465" s="22"/>
       <c r="BG465" s="22"/>
@@ -49600,6 +50072,7 @@
     <row r="466" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B466" s="19"/>
       <c r="C466" s="19"/>
+      <c r="G466" s="40"/>
       <c r="BE466" s="22"/>
       <c r="BF466" s="22"/>
       <c r="BG466" s="22"/>
@@ -49704,6 +50177,7 @@
     <row r="467" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B467" s="19"/>
       <c r="C467" s="19"/>
+      <c r="G467" s="40"/>
       <c r="BE467" s="22"/>
       <c r="BF467" s="22"/>
       <c r="BG467" s="22"/>
@@ -49808,6 +50282,7 @@
     <row r="468" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B468" s="19"/>
       <c r="C468" s="19"/>
+      <c r="G468" s="40"/>
       <c r="BE468" s="22"/>
       <c r="BF468" s="22"/>
       <c r="BG468" s="22"/>
@@ -49912,6 +50387,7 @@
     <row r="469" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B469" s="19"/>
       <c r="C469" s="19"/>
+      <c r="G469" s="40"/>
       <c r="BE469" s="22"/>
       <c r="BF469" s="22"/>
       <c r="BG469" s="22"/>
@@ -50016,6 +50492,7 @@
     <row r="470" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B470" s="19"/>
       <c r="C470" s="19"/>
+      <c r="G470" s="40"/>
       <c r="BE470" s="22"/>
       <c r="BF470" s="22"/>
       <c r="BG470" s="22"/>
@@ -50120,6 +50597,7 @@
     <row r="471" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B471" s="19"/>
       <c r="C471" s="19"/>
+      <c r="G471" s="40"/>
       <c r="BE471" s="22"/>
       <c r="BF471" s="22"/>
       <c r="BG471" s="22"/>
@@ -50224,6 +50702,7 @@
     <row r="472" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B472" s="19"/>
       <c r="C472" s="19"/>
+      <c r="G472" s="40"/>
       <c r="BE472" s="22"/>
       <c r="BF472" s="22"/>
       <c r="BG472" s="22"/>
@@ -50328,6 +50807,7 @@
     <row r="473" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B473" s="19"/>
       <c r="C473" s="19"/>
+      <c r="G473" s="40"/>
       <c r="BE473" s="22"/>
       <c r="BF473" s="22"/>
       <c r="BG473" s="22"/>
@@ -50432,6 +50912,7 @@
     <row r="474" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B474" s="19"/>
       <c r="C474" s="19"/>
+      <c r="G474" s="40"/>
       <c r="BE474" s="22"/>
       <c r="BF474" s="22"/>
       <c r="BG474" s="22"/>
@@ -50536,6 +51017,7 @@
     <row r="475" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B475" s="19"/>
       <c r="C475" s="19"/>
+      <c r="G475" s="40"/>
       <c r="BE475" s="22"/>
       <c r="BF475" s="22"/>
       <c r="BG475" s="22"/>
@@ -50640,6 +51122,7 @@
     <row r="476" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B476" s="19"/>
       <c r="C476" s="19"/>
+      <c r="G476" s="40"/>
       <c r="BE476" s="22"/>
       <c r="BF476" s="22"/>
       <c r="BG476" s="22"/>
@@ -50744,6 +51227,7 @@
     <row r="477" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B477" s="19"/>
       <c r="C477" s="19"/>
+      <c r="G477" s="40"/>
       <c r="BE477" s="22"/>
       <c r="BF477" s="22"/>
       <c r="BG477" s="22"/>
@@ -50848,6 +51332,7 @@
     <row r="478" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B478" s="19"/>
       <c r="C478" s="19"/>
+      <c r="G478" s="40"/>
       <c r="BE478" s="22"/>
       <c r="BF478" s="22"/>
       <c r="BG478" s="22"/>
@@ -50952,6 +51437,7 @@
     <row r="479" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B479" s="19"/>
       <c r="C479" s="19"/>
+      <c r="G479" s="40"/>
       <c r="BE479" s="22"/>
       <c r="BF479" s="22"/>
       <c r="BG479" s="22"/>
@@ -51056,6 +51542,7 @@
     <row r="480" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B480" s="19"/>
       <c r="C480" s="19"/>
+      <c r="G480" s="40"/>
       <c r="BE480" s="22"/>
       <c r="BF480" s="22"/>
       <c r="BG480" s="22"/>
@@ -51160,6 +51647,7 @@
     <row r="481" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B481" s="19"/>
       <c r="C481" s="19"/>
+      <c r="G481" s="40"/>
       <c r="BE481" s="22"/>
       <c r="BF481" s="22"/>
       <c r="BG481" s="22"/>
@@ -51264,6 +51752,7 @@
     <row r="482" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B482" s="19"/>
       <c r="C482" s="19"/>
+      <c r="G482" s="40"/>
       <c r="BE482" s="22"/>
       <c r="BF482" s="22"/>
       <c r="BG482" s="22"/>
@@ -51368,6 +51857,7 @@
     <row r="483" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B483" s="19"/>
       <c r="C483" s="19"/>
+      <c r="G483" s="40"/>
       <c r="BE483" s="22"/>
       <c r="BF483" s="22"/>
       <c r="BG483" s="22"/>
@@ -51472,6 +51962,7 @@
     <row r="484" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B484" s="19"/>
       <c r="C484" s="19"/>
+      <c r="G484" s="40"/>
       <c r="BE484" s="22"/>
       <c r="BF484" s="22"/>
       <c r="BG484" s="22"/>
@@ -51576,6 +52067,7 @@
     <row r="485" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B485" s="19"/>
       <c r="C485" s="19"/>
+      <c r="G485" s="40"/>
       <c r="BE485" s="22"/>
       <c r="BF485" s="22"/>
       <c r="BG485" s="22"/>
@@ -51680,6 +52172,7 @@
     <row r="486" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B486" s="19"/>
       <c r="C486" s="19"/>
+      <c r="G486" s="40"/>
       <c r="BE486" s="22"/>
       <c r="BF486" s="22"/>
       <c r="BG486" s="22"/>
@@ -51784,6 +52277,7 @@
     <row r="487" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B487" s="19"/>
       <c r="C487" s="19"/>
+      <c r="G487" s="40"/>
       <c r="BE487" s="22"/>
       <c r="BF487" s="22"/>
       <c r="BG487" s="22"/>
@@ -51888,6 +52382,7 @@
     <row r="488" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B488" s="19"/>
       <c r="C488" s="19"/>
+      <c r="G488" s="40"/>
       <c r="BE488" s="22"/>
       <c r="BF488" s="22"/>
       <c r="BG488" s="22"/>
@@ -51992,6 +52487,7 @@
     <row r="489" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B489" s="19"/>
       <c r="C489" s="19"/>
+      <c r="G489" s="40"/>
       <c r="BE489" s="22"/>
       <c r="BF489" s="22"/>
       <c r="BG489" s="22"/>
@@ -52096,6 +52592,7 @@
     <row r="490" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B490" s="19"/>
       <c r="C490" s="19"/>
+      <c r="G490" s="40"/>
       <c r="BE490" s="22"/>
       <c r="BF490" s="22"/>
       <c r="BG490" s="22"/>
@@ -52200,6 +52697,7 @@
     <row r="491" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B491" s="19"/>
       <c r="C491" s="19"/>
+      <c r="G491" s="40"/>
       <c r="BE491" s="22"/>
       <c r="BF491" s="22"/>
       <c r="BG491" s="22"/>
@@ -52304,6 +52802,7 @@
     <row r="492" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B492" s="19"/>
       <c r="C492" s="19"/>
+      <c r="G492" s="40"/>
       <c r="BE492" s="22"/>
       <c r="BF492" s="22"/>
       <c r="BG492" s="22"/>
@@ -52408,6 +52907,7 @@
     <row r="493" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B493" s="19"/>
       <c r="C493" s="19"/>
+      <c r="G493" s="40"/>
       <c r="BE493" s="22"/>
       <c r="BF493" s="22"/>
       <c r="BG493" s="22"/>
@@ -52512,6 +53012,7 @@
     <row r="494" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B494" s="19"/>
       <c r="C494" s="19"/>
+      <c r="G494" s="40"/>
       <c r="BE494" s="22"/>
       <c r="BF494" s="22"/>
       <c r="BG494" s="22"/>
@@ -52616,6 +53117,7 @@
     <row r="495" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B495" s="19"/>
       <c r="C495" s="19"/>
+      <c r="G495" s="40"/>
       <c r="BE495" s="22"/>
       <c r="BF495" s="22"/>
       <c r="BG495" s="22"/>
@@ -52720,6 +53222,7 @@
     <row r="496" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B496" s="19"/>
       <c r="C496" s="19"/>
+      <c r="G496" s="40"/>
       <c r="BE496" s="22"/>
       <c r="BF496" s="22"/>
       <c r="BG496" s="22"/>
@@ -52824,6 +53327,7 @@
     <row r="497" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B497" s="19"/>
       <c r="C497" s="19"/>
+      <c r="G497" s="40"/>
       <c r="BE497" s="22"/>
       <c r="BF497" s="22"/>
       <c r="BG497" s="22"/>
@@ -52928,6 +53432,7 @@
     <row r="498" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B498" s="19"/>
       <c r="C498" s="19"/>
+      <c r="G498" s="40"/>
       <c r="BE498" s="22"/>
       <c r="BF498" s="22"/>
       <c r="BG498" s="22"/>
@@ -53032,6 +53537,7 @@
     <row r="499" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B499" s="19"/>
       <c r="C499" s="19"/>
+      <c r="G499" s="40"/>
       <c r="BE499" s="22"/>
       <c r="BF499" s="22"/>
       <c r="BG499" s="22"/>
@@ -53136,6 +53642,7 @@
     <row r="500" spans="2:156" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B500" s="19"/>
       <c r="C500" s="19"/>
+      <c r="G500" s="40"/>
       <c r="BE500" s="22"/>
       <c r="BF500" s="22"/>
       <c r="BG500" s="22"/>
@@ -53239,11 +53746,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="EA6:EE6"/>
-    <mergeCell ref="BB6:BC6"/>
-    <mergeCell ref="BD6:BE6"/>
-    <mergeCell ref="BF6:BH6"/>
-    <mergeCell ref="AX5:BD5"/>
     <mergeCell ref="AK5:AS5"/>
     <mergeCell ref="AT5:AW5"/>
     <mergeCell ref="AC5:AJ5"/>
@@ -53253,6 +53755,11 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="D5:Z5"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="EA6:EE6"/>
+    <mergeCell ref="BB6:BC6"/>
+    <mergeCell ref="BD6:BE6"/>
+    <mergeCell ref="BF6:BH6"/>
+    <mergeCell ref="AX5:BD5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>